<commit_message>
add a tabu search method which loop to select neighborhoods. modify --config format. log stash.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/TestedParameter.xlsx
+++ b/INRC2_Simulator/log/TestedParameter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="0" windowWidth="14145" windowHeight="5115"/>
+    <workbookView xWindow="4680" yWindow="0" windowWidth="14145" windowHeight="5115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>TableSize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -67,6 +67,34 @@
   </si>
   <si>
     <t>CurrentRank</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MaxNoImprove</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0413</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0416</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0415</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0416</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0123</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -113,7 +141,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -125,6 +153,12 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -406,19 +440,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <pane xSplit="2" ySplit="12" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
+      <selection pane="bottomRight" activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="5.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -435,169 +473,238 @@
       <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5">
+        <v>9999</v>
+      </c>
+      <c r="D2" s="5">
+        <v>9999</v>
+      </c>
+      <c r="E2" s="5">
+        <v>9999</v>
+      </c>
+      <c r="F2" s="5">
+        <v>9999</v>
+      </c>
+      <c r="G2" s="5">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A3" s="2"/>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>0.5</v>
-      </c>
-      <c r="D3">
-        <v>0.5</v>
-      </c>
-      <c r="E3">
-        <v>0.8</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G4">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A6" s="2"/>
+      <c r="B6" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A7" s="2"/>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>0.5</v>
-      </c>
-      <c r="D7">
-        <v>0.8</v>
-      </c>
-      <c r="E7">
-        <v>0.8</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="2"/>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="F8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
+      <c r="G8">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="2"/>
       <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A10" s="2"/>
+      <c r="B10" t="s">
         <v>3</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A10" s="2" t="s">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="D10">
+      <c r="B11" s="3"/>
+      <c r="C11" s="5">
+        <v>3</v>
+      </c>
+      <c r="D11" s="1">
         <v>2</v>
       </c>
-      <c r="E10">
+      <c r="E11" s="1">
         <v>1</v>
       </c>
     </row>
+    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState columnSort="1" ref="C1:F9">
+  <sortState columnSort="1" ref="C1:G12">
     <sortCondition ref="C2:F2"/>
     <sortCondition ref="C3:F3"/>
     <sortCondition ref="C4:F4"/>
@@ -606,12 +713,15 @@
     <sortCondition ref="C7:F7"/>
     <sortCondition ref="C8:F8"/>
     <sortCondition ref="C9:F9"/>
+    <sortCondition ref="C10:F10"/>
   </sortState>
-  <mergeCells count="4">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A9"/>
+  <mergeCells count="6">
+    <mergeCell ref="A3:A6"/>
+    <mergeCell ref="A7:A10"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
log stash. make code more clear.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/TestedParameter.xlsx
+++ b/INRC2_Simulator/log/TestedParameter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5850" yWindow="0" windowWidth="14145" windowHeight="5115"/>
+    <workbookView xWindow="10260" yWindow="0" windowWidth="14145" windowHeight="5115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>TableSize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -94,7 +94,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0123</t>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -102,7 +114,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3</t>
+    <t>0419</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0420</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -448,53 +464,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="12" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="5.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.15">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="2">
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2">
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2">
         <v>9999</v>
@@ -503,10 +521,13 @@
         <v>9999</v>
       </c>
       <c r="G2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+        <v>9999</v>
+      </c>
+      <c r="H2" s="2">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -523,34 +544,40 @@
         <v>0</v>
       </c>
       <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>0.1</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4">
+        <v>1.2</v>
+      </c>
+      <c r="D4">
+        <v>1.6</v>
+      </c>
+      <c r="E4">
         <v>0.5</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>0.5</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>0.8</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A5" s="3"/>
       <c r="B5" t="s">
         <v>2</v>
@@ -570,8 +597,11 @@
       <c r="G5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
         <v>3</v>
@@ -591,8 +621,11 @@
       <c r="G6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -609,34 +642,40 @@
         <v>0</v>
       </c>
       <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>0.1</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" t="s">
         <v>1</v>
       </c>
       <c r="C8">
-        <v>0.5</v>
+        <v>1.2</v>
       </c>
       <c r="D8">
         <v>0.8</v>
       </c>
       <c r="E8">
+        <v>0.5</v>
+      </c>
+      <c r="F8">
         <v>0.8</v>
       </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
       <c r="G8">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+        <v>0.8</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" t="s">
         <v>2</v>
@@ -656,8 +695,11 @@
       <c r="G9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" t="s">
         <v>3</v>
@@ -677,51 +719,60 @@
       <c r="G10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.15">
+        <v>20</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
-  <sortState columnSort="1" ref="C1:G12">
-    <sortCondition ref="C2:F2"/>
-    <sortCondition ref="C3:F3"/>
-    <sortCondition ref="C4:F4"/>
-    <sortCondition ref="C5:F5"/>
-    <sortCondition ref="C6:F6"/>
-    <sortCondition ref="C7:F7"/>
-    <sortCondition ref="C8:F8"/>
-    <sortCondition ref="C9:F9"/>
-    <sortCondition ref="C10:F10"/>
+  <sortState columnSort="1" ref="C1:H12">
+    <sortCondition ref="C2:H2"/>
+    <sortCondition ref="C3:H3"/>
+    <sortCondition ref="C4:H4"/>
+    <sortCondition ref="C5:H5"/>
+    <sortCondition ref="C6:H6"/>
+    <sortCondition ref="C7:H7"/>
+    <sortCondition ref="C8:H8"/>
+    <sortCondition ref="C9:H9"/>
+    <sortCondition ref="C10:H10"/>
   </sortState>
   <mergeCells count="6">
     <mergeCell ref="A3:A6"/>

</xml_diff>

<commit_message>
bug fix on solution.rebuild (efficiency improve). log stash. run count increment.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/TestedParameter.xlsx
+++ b/INRC2_Simulator/log/TestedParameter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10260" yWindow="0" windowWidth="14145" windowHeight="5115"/>
+    <workbookView xWindow="11430" yWindow="0" windowWidth="14145" windowHeight="5115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>TableSize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -94,10 +94,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>123</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -106,19 +102,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0419</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>0420</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0421</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -464,31 +460,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="12" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>9</v>
@@ -502,8 +500,11 @@
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="I1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
@@ -526,8 +527,11 @@
       <c r="H2" s="2">
         <v>9999</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -552,8 +556,11 @@
       <c r="H3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>1</v>
@@ -576,8 +583,11 @@
       <c r="H4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A5" s="3"/>
       <c r="B5" t="s">
         <v>2</v>
@@ -600,8 +610,11 @@
       <c r="H5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
         <v>3</v>
@@ -624,8 +637,11 @@
       <c r="H6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -650,8 +666,11 @@
       <c r="H7">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" t="s">
         <v>1</v>
@@ -674,8 +693,11 @@
       <c r="H8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I8">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" t="s">
         <v>2</v>
@@ -698,8 +720,11 @@
       <c r="H9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.15">
+      <c r="I9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" t="s">
         <v>3</v>
@@ -722,32 +747,38 @@
       <c r="H10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="4" t="s">
+      <c r="I10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="5"/>
+      <c r="C11" s="2">
+        <v>716</v>
+      </c>
+      <c r="D11" s="2">
+        <v>724</v>
+      </c>
+      <c r="F11" s="2">
+        <v>764</v>
+      </c>
+      <c r="G11" s="2">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>14</v>
@@ -760,6 +791,9 @@
       </c>
       <c r="H12" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add block swap frame. new mode : BlockSwapMode. name changes.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/TestedParameter.xlsx
+++ b/INRC2_Simulator/log/TestedParameter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11430" yWindow="0" windowWidth="14145" windowHeight="5115"/>
+    <workbookView xWindow="12600" yWindow="0" windowWidth="14145" windowHeight="5115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
   <si>
     <t>TableSize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -115,6 +115,14 @@
   </si>
   <si>
     <t>0421</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BestAlgorithm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ARRCS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -460,21 +468,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="12" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="13" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomRight" activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="9" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
@@ -483,25 +490,25 @@
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
@@ -516,7 +523,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="2">
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="F2" s="2">
         <v>9999</v>
@@ -528,7 +535,7 @@
         <v>9999</v>
       </c>
       <c r="I2" s="2">
-        <v>1</v>
+        <v>9999</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.15">
@@ -554,10 +561,10 @@
         <v>0</v>
       </c>
       <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
         <v>0.1</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.15">
@@ -566,25 +573,25 @@
         <v>1</v>
       </c>
       <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
         <v>1.2</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>1.6</v>
-      </c>
-      <c r="E4">
-        <v>0.5</v>
       </c>
       <c r="F4">
         <v>0.5</v>
       </c>
       <c r="G4">
+        <v>0.5</v>
+      </c>
+      <c r="H4">
         <v>0.8</v>
       </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
       <c r="I4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.15">
@@ -664,10 +671,10 @@
         <v>0</v>
       </c>
       <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
         <v>0.1</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.15">
@@ -676,25 +683,25 @@
         <v>1</v>
       </c>
       <c r="C8">
+        <v>0.5</v>
+      </c>
+      <c r="D8">
         <v>1.2</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>0.8</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>0.5</v>
-      </c>
-      <c r="F8">
-        <v>0.8</v>
       </c>
       <c r="G8">
         <v>0.8</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="I8">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.15">
@@ -751,70 +758,98 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="5" t="s">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="2">
+      <c r="B12" s="5"/>
+      <c r="D12" s="2">
         <v>716</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E12" s="2">
         <v>724</v>
       </c>
-      <c r="F11" s="2">
+      <c r="G12" s="2">
         <v>764</v>
       </c>
-      <c r="G11" s="2">
+      <c r="H12" s="2">
         <v>721</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="4" t="s">
+    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="1" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="H13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>22</v>
-      </c>
     </row>
   </sheetData>
-  <sortState columnSort="1" ref="C1:H12">
-    <sortCondition ref="C2:H2"/>
-    <sortCondition ref="C3:H3"/>
-    <sortCondition ref="C4:H4"/>
-    <sortCondition ref="C5:H5"/>
-    <sortCondition ref="C6:H6"/>
-    <sortCondition ref="C7:H7"/>
-    <sortCondition ref="C8:H8"/>
-    <sortCondition ref="C9:H9"/>
-    <sortCondition ref="C10:H10"/>
+  <sortState columnSort="1" ref="C1:I13">
+    <sortCondition ref="C2:I2"/>
+    <sortCondition ref="C3:I3"/>
+    <sortCondition ref="C4:I4"/>
+    <sortCondition ref="C5:I5"/>
+    <sortCondition ref="C6:I6"/>
+    <sortCondition ref="C7:I7"/>
+    <sortCondition ref="C8:I8"/>
+    <sortCondition ref="C9:I9"/>
+    <sortCondition ref="C10:I10"/>
   </sortState>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A2:B2"/>
     <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
extract penalty mode setting from tryXXX implement to tryXXX interface. reduce duplicated penalty mode setting in swap. leave out calculation of another tryXXX in swap if first tryXXX fail. log stash.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/TestedParameter.xlsx
+++ b/INRC2_Simulator/log/TestedParameter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12600" yWindow="0" windowWidth="14145" windowHeight="5115"/>
+    <workbookView xWindow="13770" yWindow="0" windowWidth="14145" windowHeight="5115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>TableSize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -50,22 +50,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0123</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ModeSeq</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0123</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0123</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>CurrentRank</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -123,6 +111,10 @@
   </si>
   <si>
     <t>ARRCS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0422</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -468,13 +460,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="13" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="M15" sqref="M15"/>
+      <selection pane="bottomRight" activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -486,34 +478,34 @@
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="2">
@@ -760,36 +752,39 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="H11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B12" s="5"/>
+      <c r="C12" s="2">
+        <v>731</v>
+      </c>
       <c r="D12" s="2">
         <v>716</v>
       </c>
@@ -805,31 +800,122 @@
     </row>
     <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="I14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
+    </row>
+    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="20" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="21" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="22" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="23" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="24" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="25" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="26" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="27" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="28" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="29" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="30" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="31" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="32" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="33" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="34" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="35" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="36" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="37" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="38" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="39" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="40" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="41" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="42" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="43" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="44" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="45" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="46" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="47" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="48" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="49" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="50" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="51" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="52" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="53" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="54" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="55" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="56" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="57" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="58" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="59" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="60" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="61" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="62" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="63" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="64" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="65" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="66" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="67" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="68" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="69" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="70" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="71" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="72" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="73" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="74" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="75" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="76" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="77" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="78" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="79" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="80" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="81" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="82" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="83" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="84" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="85" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="86" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="87" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="88" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="89" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="90" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="91" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="92" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="93" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="94" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="95" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="96" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="97" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="98" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="99" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="100" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
   <sortState columnSort="1" ref="C1:I13">
     <sortCondition ref="C2:I2"/>

</xml_diff>

<commit_message>
finish block swap (without testing and adding it to ModSeq). log stash.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/TestedParameter.xlsx
+++ b/INRC2_Simulator/log/TestedParameter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13770" yWindow="0" windowWidth="14145" windowHeight="5115"/>
+    <workbookView xWindow="14940" yWindow="0" windowWidth="14145" windowHeight="5115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t>TableSize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -115,6 +115,22 @@
   </si>
   <si>
     <t>0422</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0423</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -460,13 +476,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I100"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="13" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="M8" sqref="M8"/>
+      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -476,7 +492,7 @@
     <col min="3" max="9" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -491,19 +507,25 @@
         <v>15</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
+        <v>23</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -518,10 +540,10 @@
         <v>1</v>
       </c>
       <c r="F2" s="2">
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="G2" s="2">
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="H2" s="2">
         <v>9999</v>
@@ -529,8 +551,14 @@
       <c r="I2" s="2">
         <v>9999</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J2" s="2">
+        <v>9999</v>
+      </c>
+      <c r="K2" s="2">
+        <v>9999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -547,19 +575,25 @@
         <v>0</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="G3">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
       <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>1</v>
@@ -574,19 +608,25 @@
         <v>1.6</v>
       </c>
       <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>0.5</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>0.5</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>0.8</v>
       </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="K4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5" s="3"/>
       <c r="B5" t="s">
         <v>2</v>
@@ -612,8 +652,14 @@
       <c r="I5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
         <v>3</v>
@@ -639,8 +685,14 @@
       <c r="I6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -657,19 +709,25 @@
         <v>0</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" t="s">
         <v>1</v>
@@ -684,19 +742,25 @@
         <v>0.8</v>
       </c>
       <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>0.5</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>0.8</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>0.8</v>
       </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="K8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" t="s">
         <v>2</v>
@@ -722,8 +786,14 @@
       <c r="I9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" t="s">
         <v>3</v>
@@ -749,8 +819,14 @@
       <c r="I10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -764,9 +840,6 @@
       <c r="E11" t="s">
         <v>21</v>
       </c>
-      <c r="F11" t="s">
-        <v>21</v>
-      </c>
       <c r="G11" t="s">
         <v>21</v>
       </c>
@@ -776,8 +849,14 @@
       <c r="I11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="J11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
         <v>7</v>
       </c>
@@ -792,13 +871,16 @@
         <v>724</v>
       </c>
       <c r="G12" s="2">
+        <v>748</v>
+      </c>
+      <c r="I12" s="2">
         <v>764</v>
       </c>
-      <c r="H12" s="2">
+      <c r="J12" s="2">
         <v>721</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
@@ -813,25 +895,27 @@
         <v>17</v>
       </c>
       <c r="F13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="I13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="I14" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
@@ -917,16 +1001,16 @@
     <row r="99" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="100" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <sortState columnSort="1" ref="C1:I13">
-    <sortCondition ref="C2:I2"/>
-    <sortCondition ref="C3:I3"/>
-    <sortCondition ref="C4:I4"/>
-    <sortCondition ref="C5:I5"/>
-    <sortCondition ref="C6:I6"/>
-    <sortCondition ref="C7:I7"/>
-    <sortCondition ref="C8:I8"/>
-    <sortCondition ref="C9:I9"/>
-    <sortCondition ref="C10:I10"/>
+  <sortState columnSort="1" ref="C1:K21">
+    <sortCondition ref="C2:K2"/>
+    <sortCondition ref="C3:K3"/>
+    <sortCondition ref="C4:K4"/>
+    <sortCondition ref="C5:K5"/>
+    <sortCondition ref="C6:K6"/>
+    <sortCondition ref="C7:K7"/>
+    <sortCondition ref="C8:K8"/>
+    <sortCondition ref="C9:K9"/>
+    <sortCondition ref="C10:K10"/>
   </sortState>
   <mergeCells count="7">
     <mergeCell ref="A3:A6"/>

</xml_diff>

<commit_message>
add MIN_TABU_BASE to improve the effectiveness of tabu on small instances. log stash.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/TestedParameter.xlsx
+++ b/INRC2_Simulator/log/TestedParameter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="14940" yWindow="0" windowWidth="14145" windowHeight="5115"/>
+    <workbookView xWindow="17280" yWindow="0" windowWidth="14145" windowHeight="5115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
   <si>
     <t>TableSize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -131,6 +131,19 @@
   </si>
   <si>
     <t>0423</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0424</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ARBCS
+ARRCS</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -177,7 +190,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -195,6 +208,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -476,13 +492,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K100"/>
+  <dimension ref="A1:L100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="13" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="H18" sqref="H18"/>
+      <selection pane="bottomRight" activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -492,7 +508,7 @@
     <col min="3" max="9" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -524,8 +540,11 @@
       <c r="K1" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="L1" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="5" t="s">
         <v>9</v>
       </c>
@@ -557,8 +576,11 @@
       <c r="K2" s="2">
         <v>9999</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -592,8 +614,11 @@
       <c r="K3">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>1</v>
@@ -625,8 +650,11 @@
       <c r="K4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A5" s="3"/>
       <c r="B5" t="s">
         <v>2</v>
@@ -658,8 +686,11 @@
       <c r="K5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
         <v>3</v>
@@ -691,8 +722,11 @@
       <c r="K6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -726,8 +760,11 @@
       <c r="K7">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L7">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A8" s="3"/>
       <c r="B8" t="s">
         <v>1</v>
@@ -759,8 +796,11 @@
       <c r="K8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A9" s="3"/>
       <c r="B9" t="s">
         <v>2</v>
@@ -792,8 +832,11 @@
       <c r="K9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A10" s="3"/>
       <c r="B10" t="s">
         <v>3</v>
@@ -825,8 +868,11 @@
       <c r="K10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="27" x14ac:dyDescent="0.15">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -840,6 +886,9 @@
       <c r="E11" t="s">
         <v>21</v>
       </c>
+      <c r="F11" s="6" t="s">
+        <v>29</v>
+      </c>
       <c r="G11" t="s">
         <v>21</v>
       </c>
@@ -856,7 +905,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="5" t="s">
         <v>7</v>
       </c>
@@ -870,17 +919,17 @@
       <c r="E12" s="2">
         <v>724</v>
       </c>
+      <c r="F12" s="2">
+        <v>713</v>
+      </c>
       <c r="G12" s="2">
         <v>748</v>
       </c>
-      <c r="I12" s="2">
-        <v>764</v>
-      </c>
       <c r="J12" s="2">
         <v>721</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="4" t="s">
         <v>8</v>
       </c>
@@ -912,10 +961,13 @@
       <c r="K13" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+      <c r="L13" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
new modeSeq added. update default config. log stash.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/TestedParameter.xlsx
+++ b/INRC2_Simulator/log/TestedParameter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="0" windowWidth="14145" windowHeight="5115"/>
+    <workbookView xWindow="18450" yWindow="0" windowWidth="14145" windowHeight="5115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>TableSize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -144,6 +144,30 @@
   <si>
     <t>ARBCS
 ARRCS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0425</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0426</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9AB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -201,6 +225,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -208,9 +235,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,13 +516,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L100"/>
+  <dimension ref="A1:N100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="13" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="L15" sqref="L15"/>
+      <selection pane="bottomRight" activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -508,11 +532,11 @@
     <col min="3" max="9" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="4"/>
+      <c r="B1" s="5"/>
       <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
@@ -543,12 +567,18 @@
       <c r="L1" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="5" t="s">
+      <c r="M1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="6"/>
       <c r="C2" s="2">
         <v>1</v>
       </c>
@@ -579,9 +609,15 @@
       <c r="L2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A3" s="3" t="s">
+      <c r="M2" s="2">
+        <v>1</v>
+      </c>
+      <c r="N2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
@@ -617,9 +653,15 @@
       <c r="L3">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A4" s="3"/>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -653,9 +695,15 @@
       <c r="L4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A5" s="3"/>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -689,9 +737,15 @@
       <c r="L5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A6" s="3"/>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -725,9 +779,15 @@
       <c r="L6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A7" s="3" t="s">
+      <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
@@ -763,9 +823,15 @@
       <c r="L7">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A8" s="3"/>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>1</v>
       </c>
@@ -799,9 +865,15 @@
       <c r="L8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A9" s="3"/>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>2</v>
       </c>
@@ -835,9 +907,15 @@
       <c r="L9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A10" s="3"/>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
+      <c r="A10" s="4"/>
       <c r="B10" t="s">
         <v>3</v>
       </c>
@@ -871,12 +949,18 @@
       <c r="L10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="27" x14ac:dyDescent="0.15">
-      <c r="A11" s="3" t="s">
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="27" x14ac:dyDescent="0.15">
+      <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="3"/>
+      <c r="B11" s="4"/>
       <c r="C11" t="s">
         <v>21</v>
       </c>
@@ -886,7 +970,7 @@
       <c r="E11" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="3" t="s">
         <v>29</v>
       </c>
       <c r="G11" t="s">
@@ -904,12 +988,18 @@
       <c r="K11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="5" t="s">
+      <c r="L11" t="s">
+        <v>34</v>
+      </c>
+      <c r="M11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="5"/>
+      <c r="B12" s="6"/>
       <c r="C12" s="2">
         <v>731</v>
       </c>
@@ -928,12 +1018,18 @@
       <c r="J12" s="2">
         <v>721</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="4" t="s">
+      <c r="L12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="4"/>
+      <c r="B13" s="5"/>
       <c r="C13" s="1" t="s">
         <v>19</v>
       </c>
@@ -964,10 +1060,16 @@
       <c r="L13" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+      <c r="M13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
new tabuSearch method which select single neighborhood randomly. mode sequence update. log stash.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/TestedParameter.xlsx
+++ b/INRC2_Simulator/log/TestedParameter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18450" yWindow="0" windowWidth="14145" windowHeight="5115"/>
+    <workbookView xWindow="20790" yWindow="0" windowWidth="14145" windowHeight="5115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
   <si>
     <t>TableSize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -161,6 +161,36 @@
   <si>
     <t>9AB</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0427</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>456CDEGHIJ</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>457CDEGHIJ</t>
+  </si>
+  <si>
+    <t>0428</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ARrCB</t>
   </si>
   <si>
     <t>X</t>
@@ -516,13 +546,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N100"/>
+  <dimension ref="A1:P100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="13" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="Q11" sqref="Q11"/>
+      <selection pane="bottomRight" activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -532,55 +562,61 @@
     <col min="3" max="9" width="6.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>23</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>33</v>
+        <v>23</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="2">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="D2" s="2">
         <v>1</v>
@@ -595,28 +631,34 @@
         <v>1</v>
       </c>
       <c r="H2" s="2">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1</v>
+      </c>
+      <c r="J2" s="2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1</v>
+      </c>
+      <c r="M2" s="2">
         <v>9999</v>
       </c>
-      <c r="I2" s="2">
+      <c r="N2" s="2">
         <v>9999</v>
       </c>
-      <c r="J2" s="2">
+      <c r="O2" s="2">
         <v>9999</v>
       </c>
-      <c r="K2" s="2">
+      <c r="P2" s="2">
         <v>9999</v>
       </c>
-      <c r="L2" s="2">
-        <v>1</v>
-      </c>
-      <c r="M2" s="2">
-        <v>1</v>
-      </c>
-      <c r="N2" s="2">
-        <v>1</v>
-      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -633,19 +675,19 @@
         <v>0</v>
       </c>
       <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <v>0.05</v>
-      </c>
-      <c r="G3">
-        <v>0.1</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
       </c>
       <c r="K3">
         <v>0.1</v>
@@ -659,50 +701,62 @@
       <c r="N3">
         <v>0</v>
       </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>1.2</v>
       </c>
       <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
         <v>1.2</v>
       </c>
-      <c r="E4">
+      <c r="G4">
+        <v>1.2</v>
+      </c>
+      <c r="H4">
+        <v>1.2</v>
+      </c>
+      <c r="I4">
         <v>1.6</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
         <v>0.5</v>
       </c>
-      <c r="I4">
+      <c r="N4">
         <v>0.5</v>
       </c>
-      <c r="J4">
+      <c r="O4">
         <v>0.8</v>
       </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>1.2</v>
+      <c r="P4">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>2</v>
@@ -711,7 +765,7 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -738,13 +792,19 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5">
         <v>0</v>
       </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>3</v>
@@ -785,8 +845,14 @@
       <c r="N6">
         <v>0</v>
       </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -803,19 +869,19 @@
         <v>0</v>
       </c>
       <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
         <v>0.05</v>
-      </c>
-      <c r="G7">
-        <v>0.1</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
       </c>
       <c r="K7">
         <v>0.1</v>
@@ -829,50 +895,62 @@
       <c r="N7">
         <v>0</v>
       </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0.1</v>
+      </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>1</v>
       </c>
       <c r="C8">
+        <v>1.2</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
         <v>0.5</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>1.2</v>
       </c>
-      <c r="E8">
-        <v>0.8</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
       <c r="G8">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="H8">
-        <v>0.5</v>
+        <v>1.2</v>
       </c>
       <c r="I8">
         <v>0.8</v>
       </c>
       <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0.5</v>
+      </c>
+      <c r="N8">
         <v>0.8</v>
       </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>1.2</v>
+      <c r="O8">
+        <v>0.8</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>2</v>
@@ -881,7 +959,7 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -908,13 +986,19 @@
         <v>0</v>
       </c>
       <c r="M9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N9">
         <v>0</v>
       </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A10" s="4"/>
       <c r="B10" t="s">
         <v>3</v>
@@ -955,35 +1039,38 @@
       <c r="N10">
         <v>0</v>
       </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:14" ht="27" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:16" ht="27" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="4"/>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>29</v>
+      <c r="F11" t="s">
+        <v>21</v>
       </c>
       <c r="G11" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="H11" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="I11" t="s">
         <v>21</v>
       </c>
-      <c r="J11" t="s">
-        <v>21</v>
+      <c r="J11" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="K11" t="s">
         <v>21</v>
@@ -992,84 +1079,114 @@
         <v>34</v>
       </c>
       <c r="M11" t="s">
-        <v>34</v>
+        <v>21</v>
+      </c>
+      <c r="N11" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" t="s">
+        <v>21</v>
+      </c>
+      <c r="P11" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="6"/>
-      <c r="C12" s="2">
+      <c r="D12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="2">
         <v>731</v>
       </c>
-      <c r="D12" s="2">
+      <c r="F12" s="2">
         <v>716</v>
       </c>
-      <c r="E12" s="2">
+      <c r="G12" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="2">
+        <v>629</v>
+      </c>
+      <c r="I12" s="2">
         <v>724</v>
       </c>
-      <c r="F12" s="2">
+      <c r="J12" s="2">
         <v>713</v>
       </c>
-      <c r="G12" s="2">
+      <c r="K12" s="2">
         <v>748</v>
-      </c>
-      <c r="J12" s="2">
-        <v>721</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>34</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>35</v>
+        <v>42</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O12" s="2">
+        <v>721</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="G13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>28</v>
       </c>
       <c r="M13" s="1" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>32</v>
+        <v>10</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
@@ -1155,16 +1272,16 @@
     <row r="99" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="100" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <sortState columnSort="1" ref="C1:K21">
-    <sortCondition ref="C2:K2"/>
-    <sortCondition ref="C3:K3"/>
-    <sortCondition ref="C4:K4"/>
-    <sortCondition ref="C5:K5"/>
-    <sortCondition ref="C6:K6"/>
-    <sortCondition ref="C7:K7"/>
-    <sortCondition ref="C8:K8"/>
-    <sortCondition ref="C9:K9"/>
-    <sortCondition ref="C10:K10"/>
+  <sortState columnSort="1" ref="C1:P13">
+    <sortCondition ref="C2:P2"/>
+    <sortCondition ref="C3:P3"/>
+    <sortCondition ref="C4:P4"/>
+    <sortCondition ref="C5:P5"/>
+    <sortCondition ref="C6:P6"/>
+    <sortCondition ref="C7:P7"/>
+    <sortCondition ref="C8:P8"/>
+    <sortCondition ref="C9:P9"/>
+    <sortCondition ref="C10:P10"/>
   </sortState>
   <mergeCells count="7">
     <mergeCell ref="A3:A6"/>

</xml_diff>

<commit_message>
log file format change. record iteration count and generation count. log stash.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/TestedParameter.xlsx
+++ b/INRC2_Simulator/log/TestedParameter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20790" yWindow="0" windowWidth="14145" windowHeight="5115"/>
+    <workbookView xWindow="23130" yWindow="0" windowWidth="14145" windowHeight="5115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
   <si>
     <t>TableSize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -179,13 +179,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>456CDEGHIJ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>457CDEGHIJ</t>
-  </si>
-  <si>
     <t>0428</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -198,6 +191,42 @@
   </si>
   <si>
     <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0429</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ARrCEB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0430</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -546,7 +575,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P100"/>
+  <dimension ref="A1:R100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="13" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
@@ -559,16 +588,23 @@
   <cols>
     <col min="1" max="1" width="10.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="9" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="16" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>30</v>
@@ -583,25 +619,25 @@
         <v>33</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>23</v>
@@ -609,8 +645,14 @@
       <c r="P1" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
@@ -646,10 +688,10 @@
         <v>1</v>
       </c>
       <c r="M2" s="2">
-        <v>9999</v>
+        <v>1</v>
       </c>
       <c r="N2" s="2">
-        <v>9999</v>
+        <v>2</v>
       </c>
       <c r="O2" s="2">
         <v>9999</v>
@@ -657,8 +699,14 @@
       <c r="P2" s="2">
         <v>9999</v>
       </c>
+      <c r="Q2" s="2">
+        <v>9999</v>
+      </c>
+      <c r="R2" s="2">
+        <v>9999</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
@@ -687,17 +735,17 @@
         <v>0</v>
       </c>
       <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
         <v>0.05</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>0.1</v>
       </c>
-      <c r="L3">
+      <c r="M3">
         <v>0.2</v>
       </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
       <c r="N3">
         <v>0</v>
       </c>
@@ -705,10 +753,16 @@
         <v>0</v>
       </c>
       <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" s="4"/>
       <c r="B4" t="s">
         <v>1</v>
@@ -732,11 +786,11 @@
         <v>1.2</v>
       </c>
       <c r="I4">
+        <v>1.2</v>
+      </c>
+      <c r="J4">
         <v>1.6</v>
       </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
       <c r="K4">
         <v>0</v>
       </c>
@@ -744,19 +798,25 @@
         <v>0</v>
       </c>
       <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>1.2</v>
+      </c>
+      <c r="O4">
         <v>0.5</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>0.5</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>0.8</v>
       </c>
-      <c r="P4">
+      <c r="R4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A5" s="4"/>
       <c r="B5" t="s">
         <v>2</v>
@@ -803,8 +863,14 @@
       <c r="P5">
         <v>0</v>
       </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A6" s="4"/>
       <c r="B6" t="s">
         <v>3</v>
@@ -851,8 +917,14 @@
       <c r="P6">
         <v>0</v>
       </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
         <v>4</v>
       </c>
@@ -881,17 +953,17 @@
         <v>0</v>
       </c>
       <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
         <v>0.05</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>0.1</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>0.2</v>
       </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
       <c r="N7">
         <v>0</v>
       </c>
@@ -899,10 +971,16 @@
         <v>0</v>
       </c>
       <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A8" s="4"/>
       <c r="B8" t="s">
         <v>1</v>
@@ -926,11 +1004,11 @@
         <v>1.2</v>
       </c>
       <c r="I8">
+        <v>1.2</v>
+      </c>
+      <c r="J8">
         <v>0.8</v>
       </c>
-      <c r="J8">
-        <v>0</v>
-      </c>
       <c r="K8">
         <v>0</v>
       </c>
@@ -938,19 +1016,25 @@
         <v>0</v>
       </c>
       <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>1.2</v>
+      </c>
+      <c r="O8">
         <v>0.5</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <v>0.8</v>
       </c>
-      <c r="O8">
+      <c r="Q8">
         <v>0.8</v>
       </c>
-      <c r="P8">
+      <c r="R8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A9" s="4"/>
       <c r="B9" t="s">
         <v>2</v>
@@ -997,8 +1081,14 @@
       <c r="P9">
         <v>0</v>
       </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A10" s="4"/>
       <c r="B10" t="s">
         <v>3</v>
@@ -1045,12 +1135,21 @@
       <c r="P10">
         <v>0</v>
       </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:16" ht="27" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:18" ht="27" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="4"/>
+      <c r="C11" t="s">
+        <v>43</v>
+      </c>
       <c r="D11" t="s">
         <v>34</v>
       </c>
@@ -1064,25 +1163,22 @@
         <v>36</v>
       </c>
       <c r="H11" t="s">
-        <v>41</v>
-      </c>
-      <c r="I11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" t="s">
         <v>21</v>
       </c>
-      <c r="J11" s="3" t="s">
+      <c r="K11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>21</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>34</v>
       </c>
-      <c r="M11" t="s">
-        <v>21</v>
-      </c>
       <c r="N11" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="O11" t="s">
         <v>21</v>
@@ -1090,20 +1186,29 @@
       <c r="P11" t="s">
         <v>21</v>
       </c>
+      <c r="Q11" t="s">
+        <v>21</v>
+      </c>
+      <c r="R11" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="12" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="6"/>
+      <c r="C12" s="2">
+        <v>636</v>
+      </c>
       <c r="D12" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="2">
-        <v>731</v>
-      </c>
-      <c r="F12" s="2">
-        <v>716</v>
+      <c r="E12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>36</v>
@@ -1111,38 +1216,41 @@
       <c r="H12" s="2">
         <v>629</v>
       </c>
-      <c r="I12" s="2">
-        <v>724</v>
-      </c>
-      <c r="J12" s="2">
-        <v>713</v>
-      </c>
-      <c r="K12" s="2">
-        <v>748</v>
+      <c r="J12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="L12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M12" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="N12" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="O12" s="2">
-        <v>721</v>
+      <c r="N12" s="2">
+        <v>622</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>31</v>
@@ -1160,33 +1268,39 @@
         <v>37</v>
       </c>
       <c r="I13" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="M13" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="N13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="P13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="Q13" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="R13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="14" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="15" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="16" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
@@ -1272,16 +1386,16 @@
     <row r="99" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="100" s="1" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <sortState columnSort="1" ref="C1:P13">
-    <sortCondition ref="C2:P2"/>
-    <sortCondition ref="C3:P3"/>
-    <sortCondition ref="C4:P4"/>
-    <sortCondition ref="C5:P5"/>
-    <sortCondition ref="C6:P6"/>
-    <sortCondition ref="C7:P7"/>
-    <sortCondition ref="C8:P8"/>
-    <sortCondition ref="C9:P9"/>
-    <sortCondition ref="C10:P10"/>
+  <sortState columnSort="1" ref="C1:R15">
+    <sortCondition ref="C2:R2"/>
+    <sortCondition ref="C3:R3"/>
+    <sortCondition ref="C4:R4"/>
+    <sortCondition ref="C5:R5"/>
+    <sortCondition ref="C6:R6"/>
+    <sortCondition ref="C7:R7"/>
+    <sortCondition ref="C8:R8"/>
+    <sortCondition ref="C9:R9"/>
+    <sortCondition ref="C10:R10"/>
   </sortState>
   <mergeCells count="7">
     <mergeCell ref="A3:A6"/>
@@ -1293,6 +1407,16 @@
     <mergeCell ref="A11:B11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <conditionalFormatting sqref="A12:XFD12">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFCFCFF"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
new implementation of findBestBlockSwap. new tool to analyze checkReslut which will get total objective value on the entire planning horizon. log update.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/TestedParameter.xlsx
+++ b/INRC2_Simulator/log/TestedParameter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25470" yWindow="0" windowWidth="14145" windowHeight="5115"/>
+    <workbookView xWindow="26640" yWindow="0" windowWidth="14145" windowHeight="5115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
   <si>
     <t>TableSize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -79,10 +79,6 @@
   </si>
   <si>
     <t>0416</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>123</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -159,10 +155,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>9AB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>X</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -171,34 +163,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>0427</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0428</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>X</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0427</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0428</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ARrCB</t>
-  </si>
-  <si>
     <t>X</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>0429</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ARrCEB</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>X</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0429</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ARrCEB</t>
+    <t>0430</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -206,19 +211,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>ACSEBR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>V</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>0501</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0504</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0502</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>V</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ACBR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>X</t>
+    <t>ASCBR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0505</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -226,39 +247,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0430</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ASCBR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACSEBR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0501</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0504</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0502</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>V</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -305,7 +294,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -321,14 +310,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -610,100 +602,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U100"/>
+  <dimension ref="A1:R100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="13" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="14" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="5.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="20" width="6.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="16384" width="5.625" style="1"/>
+    <col min="6" max="6" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="5.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="5"/>
+      <c r="B1" s="7"/>
       <c r="C1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>33</v>
-      </c>
       <c r="K1" s="2" t="s">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="8"/>
       <c r="C2" s="3">
         <v>0.5</v>
       </c>
@@ -738,32 +720,23 @@
         <v>1</v>
       </c>
       <c r="N2" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O2" s="3">
-        <v>1</v>
+        <v>9999</v>
       </c>
       <c r="P2" s="3">
-        <v>1</v>
+        <v>9999</v>
       </c>
       <c r="Q2" s="3">
-        <v>2</v>
+        <v>9999</v>
       </c>
       <c r="R2" s="3">
         <v>9999</v>
       </c>
-      <c r="S2" s="3">
-        <v>9999</v>
-      </c>
-      <c r="T2" s="3">
-        <v>9999</v>
-      </c>
-      <c r="U2" s="3">
-        <v>9999</v>
-      </c>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A3" s="4" t="s">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -794,41 +767,32 @@
         <v>0</v>
       </c>
       <c r="K3" s="1">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="L3" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="M3" s="1">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="N3" s="1">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>0</v>
+      </c>
+      <c r="R3" s="4">
         <v>0.1</v>
       </c>
-      <c r="P3" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>0</v>
-      </c>
-      <c r="R3" s="1">
-        <v>0</v>
-      </c>
-      <c r="S3" s="1">
-        <v>0</v>
-      </c>
-      <c r="T3" s="1">
-        <v>0</v>
-      </c>
-      <c r="U3" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A4" s="4"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A4" s="6"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -854,44 +818,35 @@
         <v>1.2</v>
       </c>
       <c r="J4" s="1">
+        <v>1.6</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
         <v>1.2</v>
       </c>
-      <c r="K4" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="L4" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="M4" s="1">
-        <v>1.6</v>
-      </c>
-      <c r="N4" s="1">
-        <v>0</v>
-      </c>
       <c r="O4" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="P4" s="1">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="Q4" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="R4" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="S4" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="T4" s="1">
         <v>0.8</v>
       </c>
-      <c r="U4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A5" s="4"/>
+      <c r="R4" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A5" s="6"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -940,21 +895,12 @@
       <c r="Q5" s="1">
         <v>0</v>
       </c>
-      <c r="R5" s="1">
-        <v>0</v>
-      </c>
-      <c r="S5" s="1">
-        <v>0</v>
-      </c>
-      <c r="T5" s="1">
-        <v>0</v>
-      </c>
-      <c r="U5" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A6" s="4"/>
+      <c r="R5" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A6" s="6"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1003,21 +949,12 @@
       <c r="Q6" s="1">
         <v>0</v>
       </c>
-      <c r="R6" s="1">
-        <v>0</v>
-      </c>
-      <c r="S6" s="1">
-        <v>0</v>
-      </c>
-      <c r="T6" s="1">
-        <v>0</v>
-      </c>
-      <c r="U6" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A7" s="4" t="s">
+      <c r="R6" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1048,41 +985,32 @@
         <v>0</v>
       </c>
       <c r="K7" s="1">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="L7" s="1">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="M7" s="1">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="N7" s="1">
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="O7" s="1">
+        <v>0</v>
+      </c>
+      <c r="P7" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="1">
+        <v>0</v>
+      </c>
+      <c r="R7" s="4">
         <v>0.1</v>
       </c>
-      <c r="P7" s="1">
-        <v>0.2</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>0</v>
-      </c>
-      <c r="R7" s="1">
-        <v>0</v>
-      </c>
-      <c r="S7" s="1">
-        <v>0</v>
-      </c>
-      <c r="T7" s="1">
-        <v>0</v>
-      </c>
-      <c r="U7" s="1">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A8" s="4"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A8" s="6"/>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
@@ -1108,44 +1036,35 @@
         <v>1.2</v>
       </c>
       <c r="J8" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+      <c r="M8" s="1">
+        <v>0</v>
+      </c>
+      <c r="N8" s="1">
         <v>1.2</v>
       </c>
-      <c r="K8" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="L8" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="M8" s="1">
+      <c r="O8" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="P8" s="1">
         <v>0.8</v>
       </c>
-      <c r="N8" s="1">
-        <v>0</v>
-      </c>
-      <c r="O8" s="1">
-        <v>0</v>
-      </c>
-      <c r="P8" s="1">
-        <v>0</v>
-      </c>
       <c r="Q8" s="1">
-        <v>1.2</v>
-      </c>
-      <c r="R8" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="S8" s="1">
         <v>0.8</v>
       </c>
-      <c r="T8" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="U8" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A9" s="4"/>
+      <c r="R8" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A9" s="6"/>
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1194,21 +1113,12 @@
       <c r="Q9" s="1">
         <v>0</v>
       </c>
-      <c r="R9" s="1">
-        <v>0</v>
-      </c>
-      <c r="S9" s="1">
-        <v>0</v>
-      </c>
-      <c r="T9" s="1">
-        <v>0</v>
-      </c>
-      <c r="U9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.15">
-      <c r="A10" s="4"/>
+      <c r="R9" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A10" s="6"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -1257,205 +1167,190 @@
       <c r="Q10" s="1">
         <v>0</v>
       </c>
-      <c r="R10" s="1">
-        <v>0</v>
-      </c>
-      <c r="S10" s="1">
-        <v>0</v>
-      </c>
-      <c r="T10" s="1">
-        <v>0</v>
-      </c>
-      <c r="U10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" ht="27" x14ac:dyDescent="0.15">
-      <c r="A11" s="4" t="s">
+      <c r="R10" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="27" x14ac:dyDescent="0.15">
+      <c r="A11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="D11" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>21</v>
-      </c>
       <c r="H11" s="1" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>39</v>
+        <v>55</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>29</v>
+        <v>32</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>47</v>
+        <v>20</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="6"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="3">
+        <v>626</v>
+      </c>
       <c r="D12" s="3">
         <v>636</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F12" s="3">
         <v>625</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H12" s="3">
         <v>622</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="3">
+        <v>624</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N12" s="3">
+        <v>622</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="J12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K12" s="3">
-        <v>629</v>
-      </c>
-      <c r="L12" s="3">
-        <v>624</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="P12" s="3" t="s">
+      <c r="G13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H14" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="I15" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="Q12" s="3">
-        <v>622</v>
-      </c>
-      <c r="R12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="S12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="T12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="U12" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="R13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="S13" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="T13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="U13" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="15" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="16" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.15"/>
+    </row>
+    <row r="16" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="I16" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="17" s="2" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="18" s="2" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="19" s="2" customFormat="1" x14ac:dyDescent="0.15"/>
@@ -1541,16 +1436,16 @@
     <row r="99" s="2" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="100" s="2" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <sortState columnSort="1" ref="C1:U15">
-    <sortCondition ref="C2:U2"/>
-    <sortCondition ref="C3:U3"/>
-    <sortCondition ref="C4:U4"/>
-    <sortCondition ref="C5:U5"/>
-    <sortCondition ref="C6:U6"/>
-    <sortCondition ref="C7:U7"/>
-    <sortCondition ref="C8:U8"/>
-    <sortCondition ref="C9:U9"/>
-    <sortCondition ref="C10:U10"/>
+  <sortState columnSort="1" ref="C1:R18">
+    <sortCondition ref="C2:R2"/>
+    <sortCondition ref="C3:R3"/>
+    <sortCondition ref="C4:R4"/>
+    <sortCondition ref="C5:R5"/>
+    <sortCondition ref="C6:R6"/>
+    <sortCondition ref="C7:R7"/>
+    <sortCondition ref="C8:R8"/>
+    <sortCondition ref="C9:R9"/>
+    <sortCondition ref="C10:R10"/>
   </sortState>
   <mergeCells count="7">
     <mergeCell ref="A3:A6"/>

</xml_diff>

<commit_message>
update max and min total assignment violation evaluation. add secondaryObjValue. log save.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/TestedParameter.xlsx
+++ b/INRC2_Simulator/log/TestedParameter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26640" yWindow="0" windowWidth="14145" windowHeight="5115"/>
+    <workbookView xWindow="27810" yWindow="0" windowWidth="14145" windowHeight="5115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
   <si>
     <t>TableSize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -248,6 +248,10 @@
   </si>
   <si>
     <t>ASCBR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -608,7 +612,7 @@
       <pane xSplit="2" ySplit="13" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="Q18" sqref="Q18"/>
+      <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1192,7 +1196,7 @@
         <v>20</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>55</v>
@@ -1246,7 +1250,7 @@
         <v>43</v>
       </c>
       <c r="H12" s="3">
-        <v>622</v>
+        <v>613</v>
       </c>
       <c r="I12" s="3">
         <v>624</v>

</xml_diff>

<commit_message>
new approach to set min and max total assign. bug fix.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/TestedParameter.xlsx
+++ b/INRC2_Simulator/log/TestedParameter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="27810" yWindow="0" windowWidth="14145" windowHeight="5115"/>
+    <workbookView xWindow="28980" yWindow="0" windowWidth="14145" windowHeight="5115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
   <si>
     <t>TableSize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -252,6 +252,10 @@
   </si>
   <si>
     <t>ACBR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0506</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -259,7 +263,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,6 +276,15 @@
       <sz val="9"/>
       <name val="宋体"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -298,7 +311,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -324,6 +337,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -612,7 +628,7 @@
       <pane xSplit="2" ySplit="13" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomRight" activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1338,7 +1354,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="9" t="s">
         <v>53</v>
       </c>
       <c r="I14" s="2" t="s">
@@ -1346,12 +1362,15 @@
       </c>
     </row>
     <row r="15" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="H15" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="I15" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="9" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new run type for simulator. (run all instances parallel)
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/TestedParameter.xlsx
+++ b/INRC2_Simulator/log/TestedParameter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28980" yWindow="0" windowWidth="14145" windowHeight="5115"/>
+    <workbookView xWindow="30150" yWindow="0" windowWidth="14145" windowHeight="5115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="59">
   <si>
     <t>TableSize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -256,6 +256,10 @@
   </si>
   <si>
     <t>0506</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0507</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -330,6 +334,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -337,9 +344,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -628,7 +632,7 @@
       <pane xSplit="2" ySplit="13" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="M21" sqref="M21"/>
+      <selection pane="bottomRight" activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -648,10 +652,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="7"/>
+      <c r="B1" s="8"/>
       <c r="C1" s="2" t="s">
         <v>47</v>
       </c>
@@ -702,10 +706,10 @@
       </c>
     </row>
     <row r="2" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="9"/>
       <c r="C2" s="3">
         <v>0.5</v>
       </c>
@@ -756,7 +760,7 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -812,7 +816,7 @@
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A4" s="6"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -866,7 +870,7 @@
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -920,7 +924,7 @@
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -974,7 +978,7 @@
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="7" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1030,7 +1034,7 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A8" s="6"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
@@ -1084,7 +1088,7 @@
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A9" s="6"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1138,7 +1142,7 @@
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A10" s="6"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -1192,10 +1196,10 @@
       </c>
     </row>
     <row r="11" spans="1:18" ht="27" x14ac:dyDescent="0.15">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="6"/>
+      <c r="B11" s="7"/>
       <c r="C11" s="1" t="s">
         <v>52</v>
       </c>
@@ -1246,10 +1250,10 @@
       </c>
     </row>
     <row r="12" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="3">
         <v>626</v>
       </c>
@@ -1300,10 +1304,10 @@
       </c>
     </row>
     <row r="13" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="7"/>
+      <c r="B13" s="8"/>
       <c r="C13" s="2" t="s">
         <v>49</v>
       </c>
@@ -1354,7 +1358,7 @@
       </c>
     </row>
     <row r="14" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="H14" s="9" t="s">
+      <c r="H14" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I14" s="2" t="s">
@@ -1370,7 +1374,10 @@
       </c>
     </row>
     <row r="16" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="I16" s="9" t="s">
+      <c r="H16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" s="6" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
input code to terminate program. perturb delta control.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/TestedParameter.xlsx
+++ b/INRC2_Simulator/log/TestedParameter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="31320" yWindow="0" windowWidth="14145" windowHeight="5115"/>
+    <workbookView xWindow="32490" yWindow="0" windowWidth="14145" windowHeight="5115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>TableSize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -62,34 +62,91 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>TSR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Improve</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BlockSwap</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BlockSwapTabu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Perturb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0516</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Neighborhood</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>NeighborhoodSelect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>TSR</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TSRACBR</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Improve</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BlockSwap</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>BlockSwapTabu</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0509</t>
-  </si>
-  <si>
-    <t>0509</t>
+    <t>R</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0516</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SCS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -101,55 +158,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Perturb</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>P</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0509</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>O</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>S</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>W</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>N</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>F</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -528,7 +537,7 @@
       <pane xSplit="2" ySplit="17" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -544,45 +553,27 @@
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>11</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
     </row>
     <row r="2" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="11" t="s">
@@ -598,33 +589,15 @@
       <c r="E2" s="8">
         <v>1</v>
       </c>
-      <c r="F2" s="8">
-        <v>1</v>
-      </c>
-      <c r="G2" s="8">
-        <v>1</v>
-      </c>
-      <c r="H2" s="8">
-        <v>1</v>
-      </c>
-      <c r="I2" s="8">
-        <v>1</v>
-      </c>
-      <c r="J2" s="8">
-        <v>1</v>
-      </c>
-      <c r="K2" s="8">
-        <v>1</v>
-      </c>
-      <c r="L2" s="8">
-        <v>1</v>
-      </c>
-      <c r="M2" s="8">
-        <v>1</v>
-      </c>
-      <c r="N2" s="8">
-        <v>1</v>
-      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
@@ -642,33 +615,15 @@
       <c r="E3" s="6">
         <v>0</v>
       </c>
-      <c r="F3" s="6">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6">
-        <v>0</v>
-      </c>
-      <c r="I3" s="6">
-        <v>0</v>
-      </c>
-      <c r="J3" s="6">
-        <v>0</v>
-      </c>
-      <c r="K3" s="6">
-        <v>0</v>
-      </c>
-      <c r="L3" s="6">
-        <v>0</v>
-      </c>
-      <c r="M3" s="6">
-        <v>0</v>
-      </c>
-      <c r="N3" s="6">
-        <v>0</v>
-      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
       <c r="R3" s="4"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.15">
@@ -677,41 +632,23 @@
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="6">
-        <v>1</v>
-      </c>
-      <c r="F4" s="6">
-        <v>1</v>
-      </c>
-      <c r="G4" s="6">
-        <v>1</v>
-      </c>
-      <c r="H4" s="6">
-        <v>1</v>
-      </c>
-      <c r="I4" s="6">
-        <v>1</v>
-      </c>
-      <c r="J4" s="6">
-        <v>1</v>
-      </c>
-      <c r="K4" s="6">
-        <v>1</v>
-      </c>
-      <c r="L4" s="6">
-        <v>1</v>
-      </c>
-      <c r="M4" s="6">
-        <v>1</v>
-      </c>
-      <c r="N4" s="6">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.15">
@@ -720,41 +657,23 @@
         <v>2</v>
       </c>
       <c r="C5" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="6">
-        <v>0</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0</v>
-      </c>
-      <c r="K5" s="6">
-        <v>0</v>
-      </c>
-      <c r="L5" s="6">
-        <v>0</v>
-      </c>
-      <c r="M5" s="6">
-        <v>0</v>
-      </c>
-      <c r="N5" s="6">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
       <c r="R5" s="4"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.15">
@@ -771,33 +690,15 @@
       <c r="E6" s="6">
         <v>0</v>
       </c>
-      <c r="F6" s="6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="6">
-        <v>0</v>
-      </c>
-      <c r="I6" s="6">
-        <v>0</v>
-      </c>
-      <c r="J6" s="6">
-        <v>0</v>
-      </c>
-      <c r="K6" s="6">
-        <v>0</v>
-      </c>
-      <c r="L6" s="6">
-        <v>0</v>
-      </c>
-      <c r="M6" s="6">
-        <v>0</v>
-      </c>
-      <c r="N6" s="6">
-        <v>0</v>
-      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
       <c r="R6" s="4"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.15">
@@ -816,33 +717,15 @@
       <c r="E7" s="6">
         <v>0</v>
       </c>
-      <c r="F7" s="6">
-        <v>0</v>
-      </c>
-      <c r="G7" s="6">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6">
-        <v>0</v>
-      </c>
-      <c r="I7" s="6">
-        <v>0</v>
-      </c>
-      <c r="J7" s="6">
-        <v>0</v>
-      </c>
-      <c r="K7" s="6">
-        <v>0</v>
-      </c>
-      <c r="L7" s="6">
-        <v>0</v>
-      </c>
-      <c r="M7" s="6">
-        <v>0</v>
-      </c>
-      <c r="N7" s="6">
-        <v>0</v>
-      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
       <c r="R7" s="4"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.15">
@@ -851,41 +734,23 @@
         <v>1</v>
       </c>
       <c r="C8" s="1">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="D8" s="6">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="E8" s="6">
-        <v>1</v>
-      </c>
-      <c r="F8" s="6">
-        <v>1</v>
-      </c>
-      <c r="G8" s="6">
-        <v>1</v>
-      </c>
-      <c r="H8" s="6">
-        <v>1</v>
-      </c>
-      <c r="I8" s="6">
-        <v>1</v>
-      </c>
-      <c r="J8" s="6">
-        <v>1</v>
-      </c>
-      <c r="K8" s="6">
-        <v>1</v>
-      </c>
-      <c r="L8" s="6">
-        <v>1</v>
-      </c>
-      <c r="M8" s="6">
-        <v>1</v>
-      </c>
-      <c r="N8" s="6">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
       <c r="R8" s="4"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.15">
@@ -900,35 +765,17 @@
         <v>0</v>
       </c>
       <c r="E9" s="6">
-        <v>0</v>
-      </c>
-      <c r="F9" s="6">
-        <v>0</v>
-      </c>
-      <c r="G9" s="6">
-        <v>0</v>
-      </c>
-      <c r="H9" s="6">
-        <v>0</v>
-      </c>
-      <c r="I9" s="6">
-        <v>0</v>
-      </c>
-      <c r="J9" s="6">
-        <v>0</v>
-      </c>
-      <c r="K9" s="6">
-        <v>0</v>
-      </c>
-      <c r="L9" s="6">
-        <v>0</v>
-      </c>
-      <c r="M9" s="6">
-        <v>0</v>
-      </c>
-      <c r="N9" s="6">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
       <c r="R9" s="4"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.15">
@@ -945,243 +792,99 @@
       <c r="E10" s="6">
         <v>0</v>
       </c>
-      <c r="F10" s="6">
-        <v>0</v>
-      </c>
-      <c r="G10" s="6">
-        <v>0</v>
-      </c>
-      <c r="H10" s="6">
-        <v>0</v>
-      </c>
-      <c r="I10" s="6">
-        <v>0</v>
-      </c>
-      <c r="J10" s="6">
-        <v>0</v>
-      </c>
-      <c r="K10" s="6">
-        <v>0</v>
-      </c>
-      <c r="L10" s="6">
-        <v>0</v>
-      </c>
-      <c r="M10" s="6">
-        <v>0</v>
-      </c>
-      <c r="N10" s="6">
-        <v>0</v>
-      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
       <c r="R10" s="4"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>10</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
     </row>
     <row r="12" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="L12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="M12" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N12" s="6" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A13" s="9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="6" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="N13" s="6" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A14" s="9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="N14" s="6" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.15">
@@ -1196,41 +899,23 @@
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="L17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="M17" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="N17" s="7" t="s">
-        <v>15</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
     </row>
     <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="E18" s="5"/>

</xml_diff>

<commit_message>
add perturb in scs. add local search after TSR find Optima.xlsx shell script update. log save.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/TestedParameter.xlsx
+++ b/INRC2_Simulator/log/TestedParameter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="32490" yWindow="0" windowWidth="14145" windowHeight="5115"/>
+    <workbookView xWindow="33660" yWindow="0" windowWidth="14145" windowHeight="5115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="37">
   <si>
     <t>TableSize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -159,6 +159,18 @@
   </si>
   <si>
     <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R(FixDelta)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACBR</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0517</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -214,7 +226,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -231,6 +243,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -537,14 +558,17 @@
       <pane xSplit="2" ySplit="17" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="E18" sqref="E18"/>
+      <selection pane="bottomRight" activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="12.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="8.5" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.5" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="14" width="5.5" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="18" width="6.5" style="1" bestFit="1" customWidth="1"/>
@@ -552,10 +576,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="13"/>
       <c r="C1" s="2" t="s">
         <v>21</v>
       </c>
@@ -565,10 +589,18 @@
       <c r="E1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+      <c r="F1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>22</v>
+      </c>
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7"/>
@@ -576,10 +608,10 @@
       <c r="N1" s="7"/>
     </row>
     <row r="2" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="11"/>
+      <c r="B2" s="14"/>
       <c r="C2" s="3">
         <v>1</v>
       </c>
@@ -589,10 +621,18 @@
       <c r="E2" s="8">
         <v>1</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="F2" s="11">
+        <v>1</v>
+      </c>
+      <c r="G2" s="11">
+        <v>1</v>
+      </c>
+      <c r="H2" s="11">
+        <v>1</v>
+      </c>
+      <c r="I2" s="11">
+        <v>1</v>
+      </c>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
@@ -600,7 +640,7 @@
       <c r="N2" s="8"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -615,10 +655,18 @@
       <c r="E3" s="6">
         <v>0</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
+      <c r="F3" s="9">
+        <v>0</v>
+      </c>
+      <c r="G3" s="9">
+        <v>0</v>
+      </c>
+      <c r="H3" s="9">
+        <v>0</v>
+      </c>
+      <c r="I3" s="9">
+        <v>0</v>
+      </c>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
@@ -627,7 +675,7 @@
       <c r="R3" s="4"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A4" s="9"/>
+      <c r="A4" s="12"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -640,10 +688,18 @@
       <c r="E4" s="6">
         <v>0</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
+      <c r="F4" s="9">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0</v>
+      </c>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
@@ -652,7 +708,7 @@
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A5" s="9"/>
+      <c r="A5" s="12"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -665,10 +721,18 @@
       <c r="E5" s="6">
         <v>1</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+      <c r="F5" s="9">
+        <v>1</v>
+      </c>
+      <c r="G5" s="9">
+        <v>1</v>
+      </c>
+      <c r="H5" s="9">
+        <v>1</v>
+      </c>
+      <c r="I5" s="9">
+        <v>1</v>
+      </c>
       <c r="J5" s="6"/>
       <c r="K5" s="6"/>
       <c r="L5" s="6"/>
@@ -677,7 +741,7 @@
       <c r="R5" s="4"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A6" s="9"/>
+      <c r="A6" s="12"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -690,10 +754,18 @@
       <c r="E6" s="6">
         <v>0</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+      <c r="F6" s="9">
+        <v>0</v>
+      </c>
+      <c r="G6" s="9">
+        <v>0</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0</v>
+      </c>
+      <c r="I6" s="9">
+        <v>0</v>
+      </c>
       <c r="J6" s="6"/>
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
@@ -702,7 +774,7 @@
       <c r="R6" s="4"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -717,10 +789,18 @@
       <c r="E7" s="6">
         <v>0</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="F7" s="9">
+        <v>0</v>
+      </c>
+      <c r="G7" s="9">
+        <v>0</v>
+      </c>
+      <c r="H7" s="9">
+        <v>0</v>
+      </c>
+      <c r="I7" s="9">
+        <v>0</v>
+      </c>
       <c r="J7" s="6"/>
       <c r="K7" s="6"/>
       <c r="L7" s="6"/>
@@ -729,7 +809,7 @@
       <c r="R7" s="4"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A8" s="9"/>
+      <c r="A8" s="12"/>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
@@ -742,10 +822,18 @@
       <c r="E8" s="6">
         <v>0</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="F8" s="9">
+        <v>0</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="H8" s="9">
+        <v>0</v>
+      </c>
+      <c r="I8" s="9">
+        <v>0</v>
+      </c>
       <c r="J8" s="6"/>
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
@@ -754,7 +842,7 @@
       <c r="R8" s="4"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A9" s="9"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
@@ -767,10 +855,18 @@
       <c r="E9" s="6">
         <v>1</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
+      <c r="F9" s="9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9">
+        <v>1</v>
+      </c>
+      <c r="H9" s="9">
+        <v>1</v>
+      </c>
+      <c r="I9" s="9">
+        <v>1</v>
+      </c>
       <c r="J9" s="6"/>
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
@@ -779,7 +875,7 @@
       <c r="R9" s="4"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A10" s="9"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -792,10 +888,18 @@
       <c r="E10" s="6">
         <v>0</v>
       </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
+      <c r="F10" s="9">
+        <v>0</v>
+      </c>
+      <c r="G10" s="9">
+        <v>0</v>
+      </c>
+      <c r="H10" s="9">
+        <v>0</v>
+      </c>
+      <c r="I10" s="9">
+        <v>0</v>
+      </c>
       <c r="J10" s="6"/>
       <c r="K10" s="6"/>
       <c r="L10" s="6"/>
@@ -804,10 +908,10 @@
       <c r="R10" s="4"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="9"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
@@ -817,10 +921,18 @@
       <c r="E11" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="F11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>23</v>
+      </c>
       <c r="J11" s="6"/>
       <c r="K11" s="6"/>
       <c r="L11" s="6"/>
@@ -828,10 +940,10 @@
       <c r="N11" s="6"/>
     </row>
     <row r="12" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="6" t="s">
         <v>16</v>
       </c>
@@ -841,12 +953,24 @@
       <c r="E12" s="6" t="s">
         <v>30</v>
       </c>
+      <c r="F12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="13" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="9"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="6" t="s">
         <v>13</v>
       </c>
@@ -856,12 +980,24 @@
       <c r="E13" s="6" t="s">
         <v>31</v>
       </c>
+      <c r="F13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="9"/>
+      <c r="B14" s="12"/>
       <c r="C14" s="6" t="s">
         <v>14</v>
       </c>
@@ -871,12 +1007,24 @@
       <c r="E14" s="6" t="s">
         <v>32</v>
       </c>
+      <c r="F14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="9"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="1" t="s">
         <v>17</v>
       </c>
@@ -886,18 +1034,30 @@
       <c r="E15" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="F15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="16" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="11"/>
+      <c r="B16" s="14"/>
     </row>
     <row r="17" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="10"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
@@ -907,9 +1067,15 @@
       <c r="E17" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
+      <c r="F17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>

</xml_diff>

<commit_message>
add BiasTabuSearch framework (not finished). optimize assist data reset. log save.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/TestedParameter.xlsx
+++ b/INRC2_Simulator/log/TestedParameter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="37170" yWindow="0" windowWidth="14145" windowHeight="5115"/>
+    <workbookView xWindow="39510" yWindow="0" windowWidth="14145" windowHeight="5115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="43">
   <si>
     <t>TableSize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -182,15 +182,19 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>TSR(NACC)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0517</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0517</t>
+    <t>0518</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0518</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TSR(RM)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TSR(RMIE)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -246,7 +250,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -290,6 +294,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -590,28 +603,31 @@
       <pane xSplit="2" ySplit="17" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="N13" sqref="N13"/>
+      <selection pane="bottomRight" activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="12.75" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="5.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="6.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="6.5" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="16384" width="5.625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="17"/>
+      <c r="B1" s="20"/>
       <c r="C1" s="2" t="s">
         <v>21</v>
       </c>
@@ -645,13 +661,18 @@
       <c r="M1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="N1" s="7"/>
+      <c r="N1" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="17" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="18"/>
+      <c r="B2" s="21"/>
       <c r="C2" s="3">
         <v>1</v>
       </c>
@@ -685,10 +706,15 @@
       <c r="M2" s="14">
         <v>1</v>
       </c>
-      <c r="N2" s="8"/>
+      <c r="N2" s="18">
+        <v>1</v>
+      </c>
+      <c r="O2" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="19" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -727,11 +753,16 @@
       <c r="M3" s="12">
         <v>0</v>
       </c>
-      <c r="N3" s="6"/>
+      <c r="N3" s="16">
+        <v>0</v>
+      </c>
+      <c r="O3" s="16">
+        <v>0</v>
+      </c>
       <c r="R3" s="4"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A4" s="16"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -768,11 +799,16 @@
       <c r="M4" s="12">
         <v>0</v>
       </c>
-      <c r="N4" s="6"/>
+      <c r="N4" s="16">
+        <v>0</v>
+      </c>
+      <c r="O4" s="16">
+        <v>0</v>
+      </c>
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A5" s="16"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -809,11 +845,16 @@
       <c r="M5" s="12">
         <v>1</v>
       </c>
-      <c r="N5" s="6"/>
+      <c r="N5" s="16">
+        <v>1</v>
+      </c>
+      <c r="O5" s="16">
+        <v>1</v>
+      </c>
       <c r="R5" s="4"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A6" s="16"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -850,11 +891,16 @@
       <c r="M6" s="12">
         <v>0</v>
       </c>
-      <c r="N6" s="6"/>
+      <c r="N6" s="16">
+        <v>0</v>
+      </c>
+      <c r="O6" s="16">
+        <v>0</v>
+      </c>
       <c r="R6" s="4"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="19" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -893,11 +939,16 @@
       <c r="M7" s="12">
         <v>0</v>
       </c>
-      <c r="N7" s="6"/>
+      <c r="N7" s="16">
+        <v>0</v>
+      </c>
+      <c r="O7" s="16">
+        <v>0</v>
+      </c>
       <c r="R7" s="4"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A8" s="16"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
@@ -934,11 +985,16 @@
       <c r="M8" s="12">
         <v>0</v>
       </c>
-      <c r="N8" s="6"/>
+      <c r="N8" s="16">
+        <v>0</v>
+      </c>
+      <c r="O8" s="16">
+        <v>0</v>
+      </c>
       <c r="R8" s="4"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A9" s="16"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
@@ -975,11 +1031,16 @@
       <c r="M9" s="12">
         <v>1</v>
       </c>
-      <c r="N9" s="6"/>
+      <c r="N9" s="16">
+        <v>1</v>
+      </c>
+      <c r="O9" s="16">
+        <v>1</v>
+      </c>
       <c r="R9" s="4"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A10" s="16"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -1016,14 +1077,19 @@
       <c r="M10" s="12">
         <v>0</v>
       </c>
-      <c r="N10" s="6"/>
+      <c r="N10" s="16">
+        <v>0</v>
+      </c>
+      <c r="O10" s="16">
+        <v>0</v>
+      </c>
       <c r="R10" s="4"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="16"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
@@ -1052,18 +1118,23 @@
         <v>38</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="N11" s="6"/>
+        <v>41</v>
+      </c>
+      <c r="N11" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="O11" s="16" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="12" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="16"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="6" t="s">
         <v>16</v>
       </c>
@@ -1097,12 +1168,18 @@
       <c r="M12" s="12" t="s">
         <v>16</v>
       </c>
+      <c r="N12" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="O12" s="16" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="13" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="16" t="s">
+      <c r="A13" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="16"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="6" t="s">
         <v>13</v>
       </c>
@@ -1136,12 +1213,18 @@
       <c r="M13" s="12" t="s">
         <v>25</v>
       </c>
+      <c r="N13" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="O13" s="16" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="14" spans="1:18" s="6" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="16"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="6" t="s">
         <v>14</v>
       </c>
@@ -1175,12 +1258,18 @@
       <c r="M14" s="12" t="s">
         <v>26</v>
       </c>
+      <c r="N14" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="O14" s="16" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.15">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="16"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="1" t="s">
         <v>17</v>
       </c>
@@ -1214,12 +1303,18 @@
       <c r="M15" s="12" t="s">
         <v>17</v>
       </c>
+      <c r="N15" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="O15" s="16" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="16" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="18"/>
+      <c r="B16" s="21"/>
       <c r="C16" s="3">
         <v>4003.2375000000006</v>
       </c>
@@ -1232,12 +1327,18 @@
       <c r="G16" s="3">
         <v>3975.2678571428573</v>
       </c>
+      <c r="J16" s="3">
+        <v>4004.7778571428576</v>
+      </c>
+      <c r="K16" s="3">
+        <v>3992.9025000000006</v>
+      </c>
     </row>
     <row r="17" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="17"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="2" t="s">
         <v>18</v>
       </c>
@@ -1253,13 +1354,17 @@
       <c r="G17" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
+      <c r="H17" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="J17" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>

</xml_diff>

<commit_message>
fix parameters. log save.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/TestedParameter.xlsx
+++ b/INRC2_Simulator/log/TestedParameter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="59400" yWindow="0" windowWidth="14145" windowHeight="5115"/>
+    <workbookView xWindow="64080" yWindow="0" windowWidth="14145" windowHeight="5115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -238,7 +238,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -342,6 +342,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -360,8 +363,119 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF53FF88"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -642,7 +756,7 @@
       <pane xSplit="2" ySplit="19" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
+      <selection pane="bottomRight" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="13.5"/>
@@ -656,10 +770,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="2" customFormat="1">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="36"/>
+      <c r="B1" s="37"/>
       <c r="C1" s="20" t="s">
         <v>17</v>
       </c>
@@ -716,10 +830,10 @@
       </c>
     </row>
     <row r="2" spans="1:20" s="3" customFormat="1">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="38"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="22">
         <v>0.5</v>
       </c>
@@ -776,7 +890,7 @@
       </c>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="36" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -838,7 +952,7 @@
       </c>
     </row>
     <row r="4" spans="1:20">
-      <c r="A4" s="35"/>
+      <c r="A4" s="36"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -898,7 +1012,7 @@
       </c>
     </row>
     <row r="5" spans="1:20">
-      <c r="A5" s="35"/>
+      <c r="A5" s="36"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
@@ -958,7 +1072,7 @@
       </c>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="35"/>
+      <c r="A6" s="36"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -1018,7 +1132,7 @@
       </c>
     </row>
     <row r="7" spans="1:20">
-      <c r="A7" s="35" t="s">
+      <c r="A7" s="36" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -1080,7 +1194,7 @@
       </c>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="35"/>
+      <c r="A8" s="36"/>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
@@ -1140,7 +1254,7 @@
       </c>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="35"/>
+      <c r="A9" s="36"/>
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1200,7 +1314,7 @@
       </c>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="35"/>
+      <c r="A10" s="36"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
@@ -1260,10 +1374,10 @@
       </c>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="35" t="s">
+      <c r="A11" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="35"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="19" t="s">
         <v>30</v>
       </c>
@@ -1320,10 +1434,10 @@
       </c>
     </row>
     <row r="12" spans="1:20" s="4" customFormat="1">
-      <c r="A12" s="35" t="s">
+      <c r="A12" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="35"/>
+      <c r="B12" s="36"/>
       <c r="C12" s="19" t="s">
         <v>13</v>
       </c>
@@ -1380,10 +1494,10 @@
       </c>
     </row>
     <row r="13" spans="1:20" s="4" customFormat="1">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="35"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="19" t="s">
         <v>18</v>
       </c>
@@ -1440,10 +1554,10 @@
       </c>
     </row>
     <row r="14" spans="1:20" s="4" customFormat="1">
-      <c r="A14" s="35" t="s">
+      <c r="A14" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="35"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="19" t="s">
         <v>19</v>
       </c>
@@ -1500,10 +1614,10 @@
       </c>
     </row>
     <row r="15" spans="1:20">
-      <c r="A15" s="35" t="s">
+      <c r="A15" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="35"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="19" t="s">
         <v>14</v>
       </c>
@@ -1560,10 +1674,10 @@
       </c>
     </row>
     <row r="16" spans="1:20" s="16" customFormat="1">
-      <c r="A16" s="35" t="s">
+      <c r="A16" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="35"/>
+      <c r="B16" s="36"/>
       <c r="C16" s="19">
         <v>8</v>
       </c>
@@ -1620,10 +1734,10 @@
       </c>
     </row>
     <row r="17" spans="1:20" s="16" customFormat="1">
-      <c r="A17" s="35" t="s">
+      <c r="A17" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="35"/>
+      <c r="B17" s="36"/>
       <c r="C17" s="19">
         <v>8</v>
       </c>
@@ -1680,21 +1794,31 @@
       </c>
     </row>
     <row r="18" spans="1:20" s="5" customFormat="1">
-      <c r="A18" s="37" t="s">
+      <c r="A18" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="37"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="31"/>
+      <c r="B18" s="38"/>
+      <c r="C18" s="21">
+        <v>3873.6160714285716</v>
+      </c>
+      <c r="D18" s="31">
+        <v>3890.8042857142859</v>
+      </c>
       <c r="E18" s="27">
         <v>3867.3660714285716</v>
       </c>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
+      <c r="F18" s="27">
+        <v>3876.9642857142858</v>
+      </c>
+      <c r="G18" s="27">
+        <v>3855.0403571428574</v>
+      </c>
       <c r="H18" s="21">
         <v>3874.1521428571432</v>
       </c>
-      <c r="I18" s="12"/>
+      <c r="I18" s="12">
+        <v>3833.6832142857143</v>
+      </c>
       <c r="J18" s="5">
         <v>3875.1567857142859</v>
       </c>
@@ -1704,12 +1828,18 @@
       <c r="L18" s="5">
         <v>3878.5721428571428</v>
       </c>
+      <c r="M18" s="5">
+        <v>3890.1785714285716</v>
+      </c>
       <c r="N18" s="5">
         <v>3896.0046428571432</v>
       </c>
       <c r="O18" s="5">
         <v>3905.335357142857</v>
       </c>
+      <c r="Q18" s="5">
+        <v>3925</v>
+      </c>
       <c r="R18" s="5">
         <v>3885.2907142857143</v>
       </c>
@@ -1721,14 +1851,14 @@
       </c>
     </row>
     <row r="19" spans="1:20" s="2" customFormat="1">
-      <c r="A19" s="36" t="s">
+      <c r="A19" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="36"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="35" t="s">
         <v>34</v>
       </c>
       <c r="E19" s="26" t="s">
@@ -1783,7 +1913,7 @@
     <row r="20" spans="1:20" s="2" customFormat="1">
       <c r="C20" s="20"/>
       <c r="D20" s="30"/>
-      <c r="E20" s="33" t="s">
+      <c r="E20" s="35" t="s">
         <v>34</v>
       </c>
       <c r="F20" s="26"/>
@@ -2523,8 +2653,8 @@
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
+        <color rgb="FF53FF88"/>
+        <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
analyzer update. log save.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/TestedParameter.xlsx
+++ b/INRC2_Simulator/log/TestedParameter.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="57060" yWindow="0" windowWidth="14145" windowHeight="5115"/>
+    <workbookView xWindow="64080" yWindow="0" windowWidth="14145" windowHeight="5115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="36">
   <si>
     <t>TableSize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -238,7 +238,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -342,14 +342,140 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF7C80"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF66FF66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF33CC33"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF53FF88"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -624,33 +750,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S106"/>
+  <dimension ref="A1:T106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="19" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="J26" sqref="J26"/>
+      <selection pane="bottomRight" activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="2" width="10.625" style="1"/>
     <col min="3" max="3" width="10.625" style="19"/>
-    <col min="4" max="6" width="10.625" style="25"/>
-    <col min="7" max="7" width="10.625" style="19"/>
-    <col min="8" max="16384" width="10.625" style="1"/>
+    <col min="4" max="4" width="10.625" style="29"/>
+    <col min="5" max="7" width="10.625" style="25"/>
+    <col min="8" max="8" width="10.625" style="19"/>
+    <col min="9" max="16384" width="10.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="2" customFormat="1">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:20" s="2" customFormat="1">
+      <c r="A1" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="30"/>
+      <c r="B1" s="37"/>
       <c r="C1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="30" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="26" t="s">
@@ -659,13 +786,13 @@
       <c r="F1" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="7" t="s">
         <v>17</v>
       </c>
       <c r="J1" s="10" t="s">
@@ -689,40 +816,43 @@
       <c r="P1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="14" t="s">
+      <c r="Q1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="17" t="s">
+      <c r="R1" s="14" t="s">
         <v>17</v>
       </c>
       <c r="S1" s="17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" s="3" customFormat="1">
-      <c r="A2" s="32" t="s">
+      <c r="T1" s="17" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" s="3" customFormat="1">
+      <c r="A2" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="32"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="22">
         <v>0.5</v>
       </c>
-      <c r="D2" s="28">
+      <c r="D2" s="32">
+        <v>0.25</v>
+      </c>
+      <c r="E2" s="28">
         <v>0.5</v>
       </c>
-      <c r="E2" s="28">
+      <c r="F2" s="28">
         <v>0.75</v>
       </c>
-      <c r="F2" s="28">
+      <c r="G2" s="28">
         <v>1</v>
       </c>
-      <c r="G2" s="22">
+      <c r="H2" s="22">
         <v>1</v>
       </c>
-      <c r="H2" s="8">
-        <v>1</v>
-      </c>
-      <c r="I2" s="11">
+      <c r="I2" s="8">
         <v>1</v>
       </c>
       <c r="J2" s="11">
@@ -746,18 +876,21 @@
       <c r="P2" s="11">
         <v>1</v>
       </c>
-      <c r="Q2" s="15">
+      <c r="Q2" s="11">
+        <v>1</v>
+      </c>
+      <c r="R2" s="15">
         <v>1.25</v>
-      </c>
-      <c r="R2" s="18">
-        <v>2</v>
       </c>
       <c r="S2" s="18">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:19">
-      <c r="A3" s="29" t="s">
+      <c r="T2" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="A3" s="36" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -766,7 +899,7 @@
       <c r="C3" s="19">
         <v>0</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="29">
         <v>0</v>
       </c>
       <c r="E3" s="25">
@@ -775,13 +908,13 @@
       <c r="F3" s="25">
         <v>0</v>
       </c>
-      <c r="G3" s="19">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6">
-        <v>0</v>
-      </c>
-      <c r="I3" s="9">
+      <c r="G3" s="25">
+        <v>0</v>
+      </c>
+      <c r="H3" s="19">
+        <v>0</v>
+      </c>
+      <c r="I3" s="6">
         <v>0</v>
       </c>
       <c r="J3" s="9">
@@ -805,25 +938,28 @@
       <c r="P3" s="9">
         <v>0</v>
       </c>
-      <c r="Q3" s="13">
-        <v>0</v>
-      </c>
-      <c r="R3" s="16">
+      <c r="Q3" s="9">
+        <v>0</v>
+      </c>
+      <c r="R3" s="13">
         <v>0</v>
       </c>
       <c r="S3" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:19">
-      <c r="A4" s="29"/>
+      <c r="T3" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
+      <c r="A4" s="36"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="19">
         <v>0</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="29">
         <v>0</v>
       </c>
       <c r="E4" s="25">
@@ -832,13 +968,13 @@
       <c r="F4" s="25">
         <v>0</v>
       </c>
-      <c r="G4" s="19">
-        <v>0</v>
-      </c>
-      <c r="H4" s="6">
-        <v>0</v>
-      </c>
-      <c r="I4" s="9">
+      <c r="G4" s="25">
+        <v>0</v>
+      </c>
+      <c r="H4" s="19">
+        <v>0</v>
+      </c>
+      <c r="I4" s="6">
         <v>0</v>
       </c>
       <c r="J4" s="9">
@@ -854,48 +990,51 @@
         <v>0</v>
       </c>
       <c r="N4" s="9">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="O4" s="9">
         <v>0.2</v>
       </c>
       <c r="P4" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="Q4" s="9">
         <v>0.5</v>
       </c>
-      <c r="Q4" s="13">
-        <v>0</v>
-      </c>
-      <c r="R4" s="16">
+      <c r="R4" s="13">
+        <v>0</v>
+      </c>
+      <c r="S4" s="16">
         <v>0.8</v>
       </c>
-      <c r="S4" s="16">
+      <c r="T4" s="16">
         <v>1.2</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
-      <c r="A5" s="29"/>
+    <row r="5" spans="1:20">
+      <c r="A5" s="36"/>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C5" s="19">
         <v>0</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="29">
         <v>0</v>
       </c>
       <c r="E5" s="25">
+        <v>0</v>
+      </c>
+      <c r="F5" s="25">
         <v>1</v>
       </c>
-      <c r="F5" s="25">
-        <v>0</v>
-      </c>
-      <c r="G5" s="19">
-        <v>0</v>
-      </c>
-      <c r="H5" s="6">
-        <v>1</v>
-      </c>
-      <c r="I5" s="9">
+      <c r="G5" s="25">
+        <v>0</v>
+      </c>
+      <c r="H5" s="19">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
         <v>1</v>
       </c>
       <c r="J5" s="9">
@@ -908,36 +1047,39 @@
         <v>1</v>
       </c>
       <c r="M5" s="9">
+        <v>1</v>
+      </c>
+      <c r="N5" s="9">
         <v>2</v>
       </c>
-      <c r="N5" s="9">
-        <v>0</v>
-      </c>
       <c r="O5" s="9">
         <v>0</v>
       </c>
       <c r="P5" s="9">
         <v>0</v>
       </c>
-      <c r="Q5" s="13">
+      <c r="Q5" s="9">
+        <v>0</v>
+      </c>
+      <c r="R5" s="13">
         <v>1</v>
       </c>
-      <c r="R5" s="16">
-        <v>0</v>
-      </c>
       <c r="S5" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:19">
-      <c r="A6" s="29"/>
+      <c r="T5" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="36"/>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C6" s="19">
         <v>0</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="29">
         <v>0</v>
       </c>
       <c r="E6" s="25">
@@ -946,13 +1088,13 @@
       <c r="F6" s="25">
         <v>0</v>
       </c>
-      <c r="G6" s="19">
-        <v>0</v>
-      </c>
-      <c r="H6" s="6">
-        <v>0</v>
-      </c>
-      <c r="I6" s="9">
+      <c r="G6" s="25">
+        <v>0</v>
+      </c>
+      <c r="H6" s="19">
+        <v>0</v>
+      </c>
+      <c r="I6" s="6">
         <v>0</v>
       </c>
       <c r="J6" s="9">
@@ -976,18 +1118,21 @@
       <c r="P6" s="9">
         <v>0</v>
       </c>
-      <c r="Q6" s="13">
-        <v>0</v>
-      </c>
-      <c r="R6" s="16">
+      <c r="Q6" s="9">
+        <v>0</v>
+      </c>
+      <c r="R6" s="13">
         <v>0</v>
       </c>
       <c r="S6" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:19">
-      <c r="A7" s="29" t="s">
+      <c r="T6" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="36" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
@@ -996,7 +1141,7 @@
       <c r="C7" s="19">
         <v>0</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="29">
         <v>0</v>
       </c>
       <c r="E7" s="25">
@@ -1005,13 +1150,13 @@
       <c r="F7" s="25">
         <v>0</v>
       </c>
-      <c r="G7" s="19">
-        <v>0</v>
-      </c>
-      <c r="H7" s="6">
-        <v>0</v>
-      </c>
-      <c r="I7" s="9">
+      <c r="G7" s="25">
+        <v>0</v>
+      </c>
+      <c r="H7" s="19">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6">
         <v>0</v>
       </c>
       <c r="J7" s="9">
@@ -1035,25 +1180,28 @@
       <c r="P7" s="9">
         <v>0</v>
       </c>
-      <c r="Q7" s="13">
-        <v>0</v>
-      </c>
-      <c r="R7" s="16">
+      <c r="Q7" s="9">
+        <v>0</v>
+      </c>
+      <c r="R7" s="13">
         <v>0</v>
       </c>
       <c r="S7" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="A8" s="29"/>
+      <c r="T7" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="36"/>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C8" s="19">
         <v>0</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="29">
         <v>0</v>
       </c>
       <c r="E8" s="25">
@@ -1062,13 +1210,13 @@
       <c r="F8" s="25">
         <v>0</v>
       </c>
-      <c r="G8" s="19">
-        <v>0</v>
-      </c>
-      <c r="H8" s="6">
-        <v>0</v>
-      </c>
-      <c r="I8" s="9">
+      <c r="G8" s="25">
+        <v>0</v>
+      </c>
+      <c r="H8" s="19">
+        <v>0</v>
+      </c>
+      <c r="I8" s="6">
         <v>0</v>
       </c>
       <c r="J8" s="9">
@@ -1078,54 +1226,57 @@
         <v>0</v>
       </c>
       <c r="L8" s="9">
+        <v>0</v>
+      </c>
+      <c r="M8" s="9">
         <v>0.2</v>
       </c>
-      <c r="M8" s="9">
-        <v>0</v>
-      </c>
       <c r="N8" s="9">
+        <v>0</v>
+      </c>
+      <c r="O8" s="9">
         <v>0.2</v>
       </c>
-      <c r="O8" s="9">
+      <c r="P8" s="9">
         <v>0.8</v>
       </c>
-      <c r="P8" s="9">
+      <c r="Q8" s="9">
         <v>0.5</v>
       </c>
-      <c r="Q8" s="13">
-        <v>0</v>
-      </c>
-      <c r="R8" s="16">
+      <c r="R8" s="13">
+        <v>0</v>
+      </c>
+      <c r="S8" s="16">
         <v>0.8</v>
       </c>
-      <c r="S8" s="16">
+      <c r="T8" s="16">
         <v>1.2</v>
       </c>
     </row>
-    <row r="9" spans="1:19">
-      <c r="A9" s="29"/>
+    <row r="9" spans="1:20">
+      <c r="A9" s="36"/>
       <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C9" s="19">
         <v>0</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="29">
         <v>0</v>
       </c>
       <c r="E9" s="25">
+        <v>0</v>
+      </c>
+      <c r="F9" s="25">
         <v>1</v>
       </c>
-      <c r="F9" s="25">
-        <v>0</v>
-      </c>
-      <c r="G9" s="19">
-        <v>0</v>
-      </c>
-      <c r="H9" s="6">
-        <v>1</v>
-      </c>
-      <c r="I9" s="9">
+      <c r="G9" s="25">
+        <v>0</v>
+      </c>
+      <c r="H9" s="19">
+        <v>0</v>
+      </c>
+      <c r="I9" s="6">
         <v>1</v>
       </c>
       <c r="J9" s="9">
@@ -1135,39 +1286,42 @@
         <v>1</v>
       </c>
       <c r="L9" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M9" s="9">
+        <v>0</v>
+      </c>
+      <c r="N9" s="9">
         <v>2</v>
       </c>
-      <c r="N9" s="9">
-        <v>0</v>
-      </c>
       <c r="O9" s="9">
         <v>0</v>
       </c>
       <c r="P9" s="9">
         <v>0</v>
       </c>
-      <c r="Q9" s="13">
+      <c r="Q9" s="9">
+        <v>0</v>
+      </c>
+      <c r="R9" s="13">
         <v>1</v>
       </c>
-      <c r="R9" s="16">
-        <v>0</v>
-      </c>
       <c r="S9" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:19">
-      <c r="A10" s="29"/>
+      <c r="T9" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
+      <c r="A10" s="36"/>
       <c r="B10" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="19">
         <v>0</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="29">
         <v>0</v>
       </c>
       <c r="E10" s="25">
@@ -1176,13 +1330,13 @@
       <c r="F10" s="25">
         <v>0</v>
       </c>
-      <c r="G10" s="19">
-        <v>0</v>
-      </c>
-      <c r="H10" s="6">
-        <v>0</v>
-      </c>
-      <c r="I10" s="9">
+      <c r="G10" s="25">
+        <v>0</v>
+      </c>
+      <c r="H10" s="19">
+        <v>0</v>
+      </c>
+      <c r="I10" s="6">
         <v>0</v>
       </c>
       <c r="J10" s="9">
@@ -1206,50 +1360,53 @@
       <c r="P10" s="9">
         <v>0</v>
       </c>
-      <c r="Q10" s="13">
-        <v>0</v>
-      </c>
-      <c r="R10" s="16">
+      <c r="Q10" s="9">
+        <v>0</v>
+      </c>
+      <c r="R10" s="13">
         <v>0</v>
       </c>
       <c r="S10" s="16">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:19">
-      <c r="A11" s="29" t="s">
+      <c r="T10" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
+      <c r="A11" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="29"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="29" t="s">
         <v>20</v>
       </c>
       <c r="E11" s="25" t="s">
         <v>20</v>
       </c>
       <c r="F11" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="H11" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="I11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="J11" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="K11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="L11" s="9" t="s">
         <v>32</v>
-      </c>
-      <c r="L11" s="9" t="s">
-        <v>20</v>
       </c>
       <c r="M11" s="9" t="s">
         <v>20</v>
@@ -1263,25 +1420,28 @@
       <c r="P11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="Q11" s="13" t="s">
+      <c r="Q11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="R11" s="16" t="s">
+      <c r="R11" s="13" t="s">
         <v>20</v>
       </c>
       <c r="S11" s="16" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" s="4" customFormat="1">
-      <c r="A12" s="29" t="s">
+      <c r="T11" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" s="4" customFormat="1">
+      <c r="A12" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="29"/>
+      <c r="B12" s="36"/>
       <c r="C12" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="25" t="s">
+      <c r="D12" s="29" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="25" t="s">
@@ -1290,13 +1450,13 @@
       <c r="F12" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="I12" s="9" t="s">
+      <c r="I12" s="6" t="s">
         <v>13</v>
       </c>
       <c r="J12" s="9" t="s">
@@ -1320,25 +1480,28 @@
       <c r="P12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="Q12" s="13" t="s">
+      <c r="Q12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="R12" s="16" t="s">
+      <c r="R12" s="13" t="s">
         <v>13</v>
       </c>
       <c r="S12" s="16" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" s="4" customFormat="1">
-      <c r="A13" s="29" t="s">
+      <c r="T12" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" s="4" customFormat="1">
+      <c r="A13" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="29"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="29" t="s">
         <v>18</v>
       </c>
       <c r="E13" s="25" t="s">
@@ -1347,13 +1510,13 @@
       <c r="F13" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="6" t="s">
         <v>18</v>
       </c>
       <c r="J13" s="9" t="s">
@@ -1377,25 +1540,28 @@
       <c r="P13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="Q13" s="13" t="s">
+      <c r="Q13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="R13" s="16" t="s">
+      <c r="R13" s="13" t="s">
         <v>18</v>
       </c>
       <c r="S13" s="16" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" s="4" customFormat="1">
-      <c r="A14" s="29" t="s">
+      <c r="T13" s="16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" s="4" customFormat="1">
+      <c r="A14" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="29"/>
+      <c r="B14" s="36"/>
       <c r="C14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="29" t="s">
         <v>19</v>
       </c>
       <c r="E14" s="25" t="s">
@@ -1404,13 +1570,13 @@
       <c r="F14" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="9" t="s">
+      <c r="I14" s="6" t="s">
         <v>19</v>
       </c>
       <c r="J14" s="9" t="s">
@@ -1434,25 +1600,28 @@
       <c r="P14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="Q14" s="13" t="s">
+      <c r="Q14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="R14" s="16" t="s">
+      <c r="R14" s="13" t="s">
         <v>19</v>
       </c>
       <c r="S14" s="16" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="A15" s="29" t="s">
+      <c r="T14" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="29"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="25" t="s">
+      <c r="D15" s="29" t="s">
         <v>14</v>
       </c>
       <c r="E15" s="25" t="s">
@@ -1461,13 +1630,13 @@
       <c r="F15" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="9" t="s">
+      <c r="I15" s="6" t="s">
         <v>14</v>
       </c>
       <c r="J15" s="9" t="s">
@@ -1491,25 +1660,28 @@
       <c r="P15" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="Q15" s="13" t="s">
+      <c r="Q15" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="R15" s="16" t="s">
+      <c r="R15" s="13" t="s">
         <v>14</v>
       </c>
       <c r="S15" s="16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" s="16" customFormat="1">
-      <c r="A16" s="29" t="s">
+      <c r="T15" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" s="16" customFormat="1">
+      <c r="A16" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="29"/>
+      <c r="B16" s="36"/>
       <c r="C16" s="19">
         <v>8</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="29">
         <v>8</v>
       </c>
       <c r="E16" s="25">
@@ -1518,29 +1690,29 @@
       <c r="F16" s="25">
         <v>8</v>
       </c>
-      <c r="G16" s="19">
+      <c r="G16" s="25">
         <v>8</v>
       </c>
-      <c r="H16" s="16">
+      <c r="H16" s="19">
         <v>8</v>
       </c>
       <c r="I16" s="16">
+        <v>8</v>
+      </c>
+      <c r="J16" s="16">
         <v>16</v>
       </c>
-      <c r="J16" s="16">
+      <c r="K16" s="16">
         <v>8</v>
       </c>
-      <c r="K16" s="16">
+      <c r="L16" s="16">
         <v>16</v>
       </c>
-      <c r="L16" s="16">
+      <c r="M16" s="16">
         <v>8</v>
       </c>
-      <c r="M16" s="16">
+      <c r="N16" s="16">
         <v>16</v>
-      </c>
-      <c r="N16" s="16">
-        <v>8</v>
       </c>
       <c r="O16" s="16">
         <v>8</v>
@@ -1549,7 +1721,7 @@
         <v>8</v>
       </c>
       <c r="Q16" s="16">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="R16" s="16">
         <v>16</v>
@@ -1557,16 +1729,19 @@
       <c r="S16" s="16">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" s="16" customFormat="1">
-      <c r="A17" s="29" t="s">
+      <c r="T16" s="16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20" s="16" customFormat="1">
+      <c r="A17" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="29"/>
+      <c r="B17" s="36"/>
       <c r="C17" s="19">
         <v>8</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="29">
         <v>8</v>
       </c>
       <c r="E17" s="25">
@@ -1575,29 +1750,29 @@
       <c r="F17" s="25">
         <v>8</v>
       </c>
-      <c r="G17" s="19">
+      <c r="G17" s="25">
         <v>8</v>
       </c>
-      <c r="H17" s="16">
+      <c r="H17" s="19">
         <v>8</v>
       </c>
       <c r="I17" s="16">
+        <v>8</v>
+      </c>
+      <c r="J17" s="16">
         <v>16</v>
       </c>
-      <c r="J17" s="16">
+      <c r="K17" s="16">
         <v>8</v>
       </c>
-      <c r="K17" s="16">
+      <c r="L17" s="16">
         <v>16</v>
       </c>
-      <c r="L17" s="16">
+      <c r="M17" s="16">
         <v>8</v>
       </c>
-      <c r="M17" s="16">
+      <c r="N17" s="16">
         <v>16</v>
-      </c>
-      <c r="N17" s="16">
-        <v>8</v>
       </c>
       <c r="O17" s="16">
         <v>8</v>
@@ -1606,7 +1781,7 @@
         <v>8</v>
       </c>
       <c r="Q17" s="16">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="R17" s="16">
         <v>16</v>
@@ -1614,719 +1789,829 @@
       <c r="S17" s="16">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" s="5" customFormat="1">
-      <c r="A18" s="31" t="s">
+      <c r="T17" s="16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" s="5" customFormat="1">
+      <c r="A18" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="31"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="27">
+      <c r="B18" s="38"/>
+      <c r="C18" s="21">
+        <v>3873.6160714285716</v>
+      </c>
+      <c r="D18" s="31">
+        <v>3890.8042857142859</v>
+      </c>
+      <c r="E18" s="27">
         <v>3867.3660714285716</v>
       </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="21">
+      <c r="F18" s="27">
+        <v>3876.9642857142858</v>
+      </c>
+      <c r="G18" s="27">
+        <v>3855.0403571428574</v>
+      </c>
+      <c r="H18" s="21">
         <v>3874.1521428571432</v>
       </c>
-      <c r="H18" s="12"/>
-      <c r="I18" s="5">
+      <c r="I18" s="12">
+        <v>3833.6832142857143</v>
+      </c>
+      <c r="J18" s="5">
         <v>3875.1567857142859</v>
       </c>
-      <c r="J18" s="5">
+      <c r="K18" s="5">
         <v>3864.9107142857142</v>
       </c>
-      <c r="K18" s="5">
+      <c r="L18" s="5">
         <v>3878.5721428571428</v>
       </c>
       <c r="M18" s="5">
+        <v>3890.1785714285716</v>
+      </c>
+      <c r="N18" s="5">
         <v>3896.0046428571432</v>
       </c>
-      <c r="N18" s="5">
+      <c r="O18" s="5">
         <v>3905.335357142857</v>
       </c>
       <c r="Q18" s="5">
+        <v>3925</v>
+      </c>
+      <c r="R18" s="5">
         <v>3885.2907142857143</v>
       </c>
-      <c r="R18" s="5">
+      <c r="S18" s="5">
         <v>4054.7546428571432</v>
       </c>
-      <c r="S18" s="5">
+      <c r="T18" s="5">
         <v>4013.8842857142859</v>
       </c>
     </row>
-    <row r="19" spans="1:19" s="2" customFormat="1">
-      <c r="A19" s="30" t="s">
+    <row r="19" spans="1:20" s="2" customFormat="1">
+      <c r="A19" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="30"/>
+      <c r="B19" s="37"/>
       <c r="C19" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="26" t="s">
+      <c r="D19" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="E19" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="F19" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="F19" s="34" t="s">
+      <c r="G19" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="H19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="H19" s="33" t="s">
+      <c r="I19" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="J19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="K19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="L19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="L19" s="24" t="s">
+      <c r="M19" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="N19" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="N19" s="2" t="s">
+      <c r="O19" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="O19" s="24" t="s">
-        <v>33</v>
       </c>
       <c r="P19" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="Q19" s="2" t="s">
+      <c r="Q19" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="R19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="R19" s="2" t="s">
+      <c r="S19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="S19" s="2" t="s">
+      <c r="T19" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:19" s="2" customFormat="1">
+    <row r="20" spans="1:20" s="2" customFormat="1">
       <c r="C20" s="20"/>
-      <c r="D20" s="33" t="s">
+      <c r="D20" s="30"/>
+      <c r="E20" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="E20" s="26"/>
       <c r="F20" s="26"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="26"/>
-      <c r="J20" s="23" t="s">
+      <c r="G20" s="26"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="26"/>
+      <c r="K20" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="K20" s="26"/>
-    </row>
-    <row r="21" spans="1:19" s="2" customFormat="1">
+      <c r="L20" s="26"/>
+    </row>
+    <row r="21" spans="1:20" s="2" customFormat="1">
       <c r="C21" s="20"/>
-      <c r="D21" s="26"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="26"/>
       <c r="F21" s="26"/>
-      <c r="G21" s="20"/>
-    </row>
-    <row r="22" spans="1:19" s="2" customFormat="1">
+      <c r="G21" s="26"/>
+      <c r="H21" s="20"/>
+    </row>
+    <row r="22" spans="1:20" s="2" customFormat="1">
       <c r="C22" s="20"/>
-      <c r="D22" s="26"/>
+      <c r="D22" s="30"/>
       <c r="E22" s="26"/>
       <c r="F22" s="26"/>
-      <c r="G22" s="20"/>
-    </row>
-    <row r="23" spans="1:19" s="2" customFormat="1">
+      <c r="G22" s="26"/>
+      <c r="H22" s="20"/>
+    </row>
+    <row r="23" spans="1:20" s="2" customFormat="1">
       <c r="C23" s="20"/>
-      <c r="D23" s="26"/>
+      <c r="D23" s="30"/>
       <c r="E23" s="26"/>
       <c r="F23" s="26"/>
-      <c r="G23" s="20"/>
-    </row>
-    <row r="24" spans="1:19" s="2" customFormat="1">
+      <c r="G23" s="26"/>
+      <c r="H23" s="20"/>
+    </row>
+    <row r="24" spans="1:20" s="2" customFormat="1">
       <c r="C24" s="20"/>
-      <c r="D24" s="26"/>
+      <c r="D24" s="30"/>
       <c r="E24" s="26"/>
       <c r="F24" s="26"/>
-      <c r="G24" s="20"/>
-    </row>
-    <row r="25" spans="1:19" s="2" customFormat="1">
+      <c r="G24" s="26"/>
+      <c r="H24" s="20"/>
+    </row>
+    <row r="25" spans="1:20" s="2" customFormat="1">
       <c r="C25" s="20"/>
-      <c r="D25" s="26"/>
+      <c r="D25" s="30"/>
       <c r="E25" s="26"/>
       <c r="F25" s="26"/>
-      <c r="G25" s="20"/>
-    </row>
-    <row r="26" spans="1:19" s="2" customFormat="1">
+      <c r="G25" s="26"/>
+      <c r="H25" s="20"/>
+    </row>
+    <row r="26" spans="1:20" s="2" customFormat="1">
       <c r="C26" s="20"/>
-      <c r="D26" s="26"/>
+      <c r="D26" s="30"/>
       <c r="E26" s="26"/>
       <c r="F26" s="26"/>
-      <c r="G26" s="20"/>
-    </row>
-    <row r="27" spans="1:19" s="2" customFormat="1">
+      <c r="G26" s="26"/>
+      <c r="H26" s="20"/>
+    </row>
+    <row r="27" spans="1:20" s="2" customFormat="1">
       <c r="C27" s="20"/>
-      <c r="D27" s="26"/>
+      <c r="D27" s="30"/>
       <c r="E27" s="26"/>
       <c r="F27" s="26"/>
-      <c r="G27" s="20"/>
-    </row>
-    <row r="28" spans="1:19" s="2" customFormat="1">
+      <c r="G27" s="26"/>
+      <c r="H27" s="20"/>
+    </row>
+    <row r="28" spans="1:20" s="2" customFormat="1">
       <c r="C28" s="20"/>
-      <c r="D28" s="26"/>
+      <c r="D28" s="30"/>
       <c r="E28" s="26"/>
       <c r="F28" s="26"/>
-      <c r="G28" s="20"/>
-    </row>
-    <row r="29" spans="1:19" s="2" customFormat="1">
+      <c r="G28" s="26"/>
+      <c r="H28" s="20"/>
+    </row>
+    <row r="29" spans="1:20" s="2" customFormat="1">
       <c r="C29" s="20"/>
-      <c r="D29" s="26"/>
+      <c r="D29" s="30"/>
       <c r="E29" s="26"/>
       <c r="F29" s="26"/>
-      <c r="G29" s="20"/>
-    </row>
-    <row r="30" spans="1:19" s="2" customFormat="1">
+      <c r="G29" s="26"/>
+      <c r="H29" s="20"/>
+    </row>
+    <row r="30" spans="1:20" s="2" customFormat="1">
       <c r="C30" s="20"/>
-      <c r="D30" s="26"/>
+      <c r="D30" s="30"/>
       <c r="E30" s="26"/>
       <c r="F30" s="26"/>
-      <c r="G30" s="20"/>
-    </row>
-    <row r="31" spans="1:19" s="2" customFormat="1">
+      <c r="G30" s="26"/>
+      <c r="H30" s="20"/>
+    </row>
+    <row r="31" spans="1:20" s="2" customFormat="1">
       <c r="C31" s="20"/>
-      <c r="D31" s="26"/>
+      <c r="D31" s="30"/>
       <c r="E31" s="26"/>
       <c r="F31" s="26"/>
-      <c r="G31" s="20"/>
-    </row>
-    <row r="32" spans="1:19" s="2" customFormat="1">
+      <c r="G31" s="26"/>
+      <c r="H31" s="20"/>
+    </row>
+    <row r="32" spans="1:20" s="2" customFormat="1">
       <c r="C32" s="20"/>
-      <c r="D32" s="26"/>
+      <c r="D32" s="30"/>
       <c r="E32" s="26"/>
       <c r="F32" s="26"/>
-      <c r="G32" s="20"/>
-    </row>
-    <row r="33" spans="3:7" s="2" customFormat="1">
+      <c r="G32" s="26"/>
+      <c r="H32" s="20"/>
+    </row>
+    <row r="33" spans="3:8" s="2" customFormat="1">
       <c r="C33" s="20"/>
-      <c r="D33" s="26"/>
+      <c r="D33" s="30"/>
       <c r="E33" s="26"/>
       <c r="F33" s="26"/>
-      <c r="G33" s="20"/>
-    </row>
-    <row r="34" spans="3:7" s="2" customFormat="1">
+      <c r="G33" s="26"/>
+      <c r="H33" s="20"/>
+    </row>
+    <row r="34" spans="3:8" s="2" customFormat="1">
       <c r="C34" s="20"/>
-      <c r="D34" s="26"/>
+      <c r="D34" s="30"/>
       <c r="E34" s="26"/>
       <c r="F34" s="26"/>
-      <c r="G34" s="20"/>
-    </row>
-    <row r="35" spans="3:7" s="2" customFormat="1">
+      <c r="G34" s="26"/>
+      <c r="H34" s="20"/>
+    </row>
+    <row r="35" spans="3:8" s="2" customFormat="1">
       <c r="C35" s="20"/>
-      <c r="D35" s="26"/>
+      <c r="D35" s="30"/>
       <c r="E35" s="26"/>
       <c r="F35" s="26"/>
-      <c r="G35" s="20"/>
-    </row>
-    <row r="36" spans="3:7" s="2" customFormat="1">
+      <c r="G35" s="26"/>
+      <c r="H35" s="20"/>
+    </row>
+    <row r="36" spans="3:8" s="2" customFormat="1">
       <c r="C36" s="20"/>
-      <c r="D36" s="26"/>
+      <c r="D36" s="30"/>
       <c r="E36" s="26"/>
       <c r="F36" s="26"/>
-      <c r="G36" s="20"/>
-    </row>
-    <row r="37" spans="3:7" s="2" customFormat="1">
+      <c r="G36" s="26"/>
+      <c r="H36" s="20"/>
+    </row>
+    <row r="37" spans="3:8" s="2" customFormat="1">
       <c r="C37" s="20"/>
-      <c r="D37" s="26"/>
+      <c r="D37" s="30"/>
       <c r="E37" s="26"/>
       <c r="F37" s="26"/>
-      <c r="G37" s="20"/>
-    </row>
-    <row r="38" spans="3:7" s="2" customFormat="1">
+      <c r="G37" s="26"/>
+      <c r="H37" s="20"/>
+    </row>
+    <row r="38" spans="3:8" s="2" customFormat="1">
       <c r="C38" s="20"/>
-      <c r="D38" s="26"/>
+      <c r="D38" s="30"/>
       <c r="E38" s="26"/>
       <c r="F38" s="26"/>
-      <c r="G38" s="20"/>
-    </row>
-    <row r="39" spans="3:7" s="2" customFormat="1">
+      <c r="G38" s="26"/>
+      <c r="H38" s="20"/>
+    </row>
+    <row r="39" spans="3:8" s="2" customFormat="1">
       <c r="C39" s="20"/>
-      <c r="D39" s="26"/>
+      <c r="D39" s="30"/>
       <c r="E39" s="26"/>
       <c r="F39" s="26"/>
-      <c r="G39" s="20"/>
-    </row>
-    <row r="40" spans="3:7" s="2" customFormat="1">
+      <c r="G39" s="26"/>
+      <c r="H39" s="20"/>
+    </row>
+    <row r="40" spans="3:8" s="2" customFormat="1">
       <c r="C40" s="20"/>
-      <c r="D40" s="26"/>
+      <c r="D40" s="30"/>
       <c r="E40" s="26"/>
       <c r="F40" s="26"/>
-      <c r="G40" s="20"/>
-    </row>
-    <row r="41" spans="3:7" s="2" customFormat="1">
+      <c r="G40" s="26"/>
+      <c r="H40" s="20"/>
+    </row>
+    <row r="41" spans="3:8" s="2" customFormat="1">
       <c r="C41" s="20"/>
-      <c r="D41" s="26"/>
+      <c r="D41" s="30"/>
       <c r="E41" s="26"/>
       <c r="F41" s="26"/>
-      <c r="G41" s="20"/>
-    </row>
-    <row r="42" spans="3:7" s="2" customFormat="1">
+      <c r="G41" s="26"/>
+      <c r="H41" s="20"/>
+    </row>
+    <row r="42" spans="3:8" s="2" customFormat="1">
       <c r="C42" s="20"/>
-      <c r="D42" s="26"/>
+      <c r="D42" s="30"/>
       <c r="E42" s="26"/>
       <c r="F42" s="26"/>
-      <c r="G42" s="20"/>
-    </row>
-    <row r="43" spans="3:7" s="2" customFormat="1">
+      <c r="G42" s="26"/>
+      <c r="H42" s="20"/>
+    </row>
+    <row r="43" spans="3:8" s="2" customFormat="1">
       <c r="C43" s="20"/>
-      <c r="D43" s="26"/>
+      <c r="D43" s="30"/>
       <c r="E43" s="26"/>
       <c r="F43" s="26"/>
-      <c r="G43" s="20"/>
-    </row>
-    <row r="44" spans="3:7" s="2" customFormat="1">
+      <c r="G43" s="26"/>
+      <c r="H43" s="20"/>
+    </row>
+    <row r="44" spans="3:8" s="2" customFormat="1">
       <c r="C44" s="20"/>
-      <c r="D44" s="26"/>
+      <c r="D44" s="30"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
-      <c r="G44" s="20"/>
-    </row>
-    <row r="45" spans="3:7" s="2" customFormat="1">
+      <c r="G44" s="26"/>
+      <c r="H44" s="20"/>
+    </row>
+    <row r="45" spans="3:8" s="2" customFormat="1">
       <c r="C45" s="20"/>
-      <c r="D45" s="26"/>
+      <c r="D45" s="30"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
-      <c r="G45" s="20"/>
-    </row>
-    <row r="46" spans="3:7" s="2" customFormat="1">
+      <c r="G45" s="26"/>
+      <c r="H45" s="20"/>
+    </row>
+    <row r="46" spans="3:8" s="2" customFormat="1">
       <c r="C46" s="20"/>
-      <c r="D46" s="26"/>
+      <c r="D46" s="30"/>
       <c r="E46" s="26"/>
       <c r="F46" s="26"/>
-      <c r="G46" s="20"/>
-    </row>
-    <row r="47" spans="3:7" s="2" customFormat="1">
+      <c r="G46" s="26"/>
+      <c r="H46" s="20"/>
+    </row>
+    <row r="47" spans="3:8" s="2" customFormat="1">
       <c r="C47" s="20"/>
-      <c r="D47" s="26"/>
+      <c r="D47" s="30"/>
       <c r="E47" s="26"/>
       <c r="F47" s="26"/>
-      <c r="G47" s="20"/>
-    </row>
-    <row r="48" spans="3:7" s="2" customFormat="1">
+      <c r="G47" s="26"/>
+      <c r="H47" s="20"/>
+    </row>
+    <row r="48" spans="3:8" s="2" customFormat="1">
       <c r="C48" s="20"/>
-      <c r="D48" s="26"/>
+      <c r="D48" s="30"/>
       <c r="E48" s="26"/>
       <c r="F48" s="26"/>
-      <c r="G48" s="20"/>
-    </row>
-    <row r="49" spans="3:7" s="2" customFormat="1">
+      <c r="G48" s="26"/>
+      <c r="H48" s="20"/>
+    </row>
+    <row r="49" spans="3:8" s="2" customFormat="1">
       <c r="C49" s="20"/>
-      <c r="D49" s="26"/>
+      <c r="D49" s="30"/>
       <c r="E49" s="26"/>
       <c r="F49" s="26"/>
-      <c r="G49" s="20"/>
-    </row>
-    <row r="50" spans="3:7" s="2" customFormat="1">
+      <c r="G49" s="26"/>
+      <c r="H49" s="20"/>
+    </row>
+    <row r="50" spans="3:8" s="2" customFormat="1">
       <c r="C50" s="20"/>
-      <c r="D50" s="26"/>
+      <c r="D50" s="30"/>
       <c r="E50" s="26"/>
       <c r="F50" s="26"/>
-      <c r="G50" s="20"/>
-    </row>
-    <row r="51" spans="3:7" s="2" customFormat="1">
+      <c r="G50" s="26"/>
+      <c r="H50" s="20"/>
+    </row>
+    <row r="51" spans="3:8" s="2" customFormat="1">
       <c r="C51" s="20"/>
-      <c r="D51" s="26"/>
+      <c r="D51" s="30"/>
       <c r="E51" s="26"/>
       <c r="F51" s="26"/>
-      <c r="G51" s="20"/>
-    </row>
-    <row r="52" spans="3:7" s="2" customFormat="1">
+      <c r="G51" s="26"/>
+      <c r="H51" s="20"/>
+    </row>
+    <row r="52" spans="3:8" s="2" customFormat="1">
       <c r="C52" s="20"/>
-      <c r="D52" s="26"/>
+      <c r="D52" s="30"/>
       <c r="E52" s="26"/>
       <c r="F52" s="26"/>
-      <c r="G52" s="20"/>
-    </row>
-    <row r="53" spans="3:7" s="2" customFormat="1">
+      <c r="G52" s="26"/>
+      <c r="H52" s="20"/>
+    </row>
+    <row r="53" spans="3:8" s="2" customFormat="1">
       <c r="C53" s="20"/>
-      <c r="D53" s="26"/>
+      <c r="D53" s="30"/>
       <c r="E53" s="26"/>
       <c r="F53" s="26"/>
-      <c r="G53" s="20"/>
-    </row>
-    <row r="54" spans="3:7" s="2" customFormat="1">
+      <c r="G53" s="26"/>
+      <c r="H53" s="20"/>
+    </row>
+    <row r="54" spans="3:8" s="2" customFormat="1">
       <c r="C54" s="20"/>
-      <c r="D54" s="26"/>
+      <c r="D54" s="30"/>
       <c r="E54" s="26"/>
       <c r="F54" s="26"/>
-      <c r="G54" s="20"/>
-    </row>
-    <row r="55" spans="3:7" s="2" customFormat="1">
+      <c r="G54" s="26"/>
+      <c r="H54" s="20"/>
+    </row>
+    <row r="55" spans="3:8" s="2" customFormat="1">
       <c r="C55" s="20"/>
-      <c r="D55" s="26"/>
+      <c r="D55" s="30"/>
       <c r="E55" s="26"/>
       <c r="F55" s="26"/>
-      <c r="G55" s="20"/>
-    </row>
-    <row r="56" spans="3:7" s="2" customFormat="1">
+      <c r="G55" s="26"/>
+      <c r="H55" s="20"/>
+    </row>
+    <row r="56" spans="3:8" s="2" customFormat="1">
       <c r="C56" s="20"/>
-      <c r="D56" s="26"/>
+      <c r="D56" s="30"/>
       <c r="E56" s="26"/>
       <c r="F56" s="26"/>
-      <c r="G56" s="20"/>
-    </row>
-    <row r="57" spans="3:7" s="2" customFormat="1">
+      <c r="G56" s="26"/>
+      <c r="H56" s="20"/>
+    </row>
+    <row r="57" spans="3:8" s="2" customFormat="1">
       <c r="C57" s="20"/>
-      <c r="D57" s="26"/>
+      <c r="D57" s="30"/>
       <c r="E57" s="26"/>
       <c r="F57" s="26"/>
-      <c r="G57" s="20"/>
-    </row>
-    <row r="58" spans="3:7" s="2" customFormat="1">
+      <c r="G57" s="26"/>
+      <c r="H57" s="20"/>
+    </row>
+    <row r="58" spans="3:8" s="2" customFormat="1">
       <c r="C58" s="20"/>
-      <c r="D58" s="26"/>
+      <c r="D58" s="30"/>
       <c r="E58" s="26"/>
       <c r="F58" s="26"/>
-      <c r="G58" s="20"/>
-    </row>
-    <row r="59" spans="3:7" s="2" customFormat="1">
+      <c r="G58" s="26"/>
+      <c r="H58" s="20"/>
+    </row>
+    <row r="59" spans="3:8" s="2" customFormat="1">
       <c r="C59" s="20"/>
-      <c r="D59" s="26"/>
+      <c r="D59" s="30"/>
       <c r="E59" s="26"/>
       <c r="F59" s="26"/>
-      <c r="G59" s="20"/>
-    </row>
-    <row r="60" spans="3:7" s="2" customFormat="1">
+      <c r="G59" s="26"/>
+      <c r="H59" s="20"/>
+    </row>
+    <row r="60" spans="3:8" s="2" customFormat="1">
       <c r="C60" s="20"/>
-      <c r="D60" s="26"/>
+      <c r="D60" s="30"/>
       <c r="E60" s="26"/>
       <c r="F60" s="26"/>
-      <c r="G60" s="20"/>
-    </row>
-    <row r="61" spans="3:7" s="2" customFormat="1">
+      <c r="G60" s="26"/>
+      <c r="H60" s="20"/>
+    </row>
+    <row r="61" spans="3:8" s="2" customFormat="1">
       <c r="C61" s="20"/>
-      <c r="D61" s="26"/>
+      <c r="D61" s="30"/>
       <c r="E61" s="26"/>
       <c r="F61" s="26"/>
-      <c r="G61" s="20"/>
-    </row>
-    <row r="62" spans="3:7" s="2" customFormat="1">
+      <c r="G61" s="26"/>
+      <c r="H61" s="20"/>
+    </row>
+    <row r="62" spans="3:8" s="2" customFormat="1">
       <c r="C62" s="20"/>
-      <c r="D62" s="26"/>
+      <c r="D62" s="30"/>
       <c r="E62" s="26"/>
       <c r="F62" s="26"/>
-      <c r="G62" s="20"/>
-    </row>
-    <row r="63" spans="3:7" s="2" customFormat="1">
+      <c r="G62" s="26"/>
+      <c r="H62" s="20"/>
+    </row>
+    <row r="63" spans="3:8" s="2" customFormat="1">
       <c r="C63" s="20"/>
-      <c r="D63" s="26"/>
+      <c r="D63" s="30"/>
       <c r="E63" s="26"/>
       <c r="F63" s="26"/>
-      <c r="G63" s="20"/>
-    </row>
-    <row r="64" spans="3:7" s="2" customFormat="1">
+      <c r="G63" s="26"/>
+      <c r="H63" s="20"/>
+    </row>
+    <row r="64" spans="3:8" s="2" customFormat="1">
       <c r="C64" s="20"/>
-      <c r="D64" s="26"/>
+      <c r="D64" s="30"/>
       <c r="E64" s="26"/>
       <c r="F64" s="26"/>
-      <c r="G64" s="20"/>
-    </row>
-    <row r="65" spans="3:7" s="2" customFormat="1">
+      <c r="G64" s="26"/>
+      <c r="H64" s="20"/>
+    </row>
+    <row r="65" spans="3:8" s="2" customFormat="1">
       <c r="C65" s="20"/>
-      <c r="D65" s="26"/>
+      <c r="D65" s="30"/>
       <c r="E65" s="26"/>
       <c r="F65" s="26"/>
-      <c r="G65" s="20"/>
-    </row>
-    <row r="66" spans="3:7" s="2" customFormat="1">
+      <c r="G65" s="26"/>
+      <c r="H65" s="20"/>
+    </row>
+    <row r="66" spans="3:8" s="2" customFormat="1">
       <c r="C66" s="20"/>
-      <c r="D66" s="26"/>
+      <c r="D66" s="30"/>
       <c r="E66" s="26"/>
       <c r="F66" s="26"/>
-      <c r="G66" s="20"/>
-    </row>
-    <row r="67" spans="3:7" s="2" customFormat="1">
+      <c r="G66" s="26"/>
+      <c r="H66" s="20"/>
+    </row>
+    <row r="67" spans="3:8" s="2" customFormat="1">
       <c r="C67" s="20"/>
-      <c r="D67" s="26"/>
+      <c r="D67" s="30"/>
       <c r="E67" s="26"/>
       <c r="F67" s="26"/>
-      <c r="G67" s="20"/>
-    </row>
-    <row r="68" spans="3:7" s="2" customFormat="1">
+      <c r="G67" s="26"/>
+      <c r="H67" s="20"/>
+    </row>
+    <row r="68" spans="3:8" s="2" customFormat="1">
       <c r="C68" s="20"/>
-      <c r="D68" s="26"/>
+      <c r="D68" s="30"/>
       <c r="E68" s="26"/>
       <c r="F68" s="26"/>
-      <c r="G68" s="20"/>
-    </row>
-    <row r="69" spans="3:7" s="2" customFormat="1">
+      <c r="G68" s="26"/>
+      <c r="H68" s="20"/>
+    </row>
+    <row r="69" spans="3:8" s="2" customFormat="1">
       <c r="C69" s="20"/>
-      <c r="D69" s="26"/>
+      <c r="D69" s="30"/>
       <c r="E69" s="26"/>
       <c r="F69" s="26"/>
-      <c r="G69" s="20"/>
-    </row>
-    <row r="70" spans="3:7" s="2" customFormat="1">
+      <c r="G69" s="26"/>
+      <c r="H69" s="20"/>
+    </row>
+    <row r="70" spans="3:8" s="2" customFormat="1">
       <c r="C70" s="20"/>
-      <c r="D70" s="26"/>
+      <c r="D70" s="30"/>
       <c r="E70" s="26"/>
       <c r="F70" s="26"/>
-      <c r="G70" s="20"/>
-    </row>
-    <row r="71" spans="3:7" s="2" customFormat="1">
+      <c r="G70" s="26"/>
+      <c r="H70" s="20"/>
+    </row>
+    <row r="71" spans="3:8" s="2" customFormat="1">
       <c r="C71" s="20"/>
-      <c r="D71" s="26"/>
+      <c r="D71" s="30"/>
       <c r="E71" s="26"/>
       <c r="F71" s="26"/>
-      <c r="G71" s="20"/>
-    </row>
-    <row r="72" spans="3:7" s="2" customFormat="1">
+      <c r="G71" s="26"/>
+      <c r="H71" s="20"/>
+    </row>
+    <row r="72" spans="3:8" s="2" customFormat="1">
       <c r="C72" s="20"/>
-      <c r="D72" s="26"/>
+      <c r="D72" s="30"/>
       <c r="E72" s="26"/>
       <c r="F72" s="26"/>
-      <c r="G72" s="20"/>
-    </row>
-    <row r="73" spans="3:7" s="2" customFormat="1">
+      <c r="G72" s="26"/>
+      <c r="H72" s="20"/>
+    </row>
+    <row r="73" spans="3:8" s="2" customFormat="1">
       <c r="C73" s="20"/>
-      <c r="D73" s="26"/>
+      <c r="D73" s="30"/>
       <c r="E73" s="26"/>
       <c r="F73" s="26"/>
-      <c r="G73" s="20"/>
-    </row>
-    <row r="74" spans="3:7" s="2" customFormat="1">
+      <c r="G73" s="26"/>
+      <c r="H73" s="20"/>
+    </row>
+    <row r="74" spans="3:8" s="2" customFormat="1">
       <c r="C74" s="20"/>
-      <c r="D74" s="26"/>
+      <c r="D74" s="30"/>
       <c r="E74" s="26"/>
       <c r="F74" s="26"/>
-      <c r="G74" s="20"/>
-    </row>
-    <row r="75" spans="3:7" s="2" customFormat="1">
+      <c r="G74" s="26"/>
+      <c r="H74" s="20"/>
+    </row>
+    <row r="75" spans="3:8" s="2" customFormat="1">
       <c r="C75" s="20"/>
-      <c r="D75" s="26"/>
+      <c r="D75" s="30"/>
       <c r="E75" s="26"/>
       <c r="F75" s="26"/>
-      <c r="G75" s="20"/>
-    </row>
-    <row r="76" spans="3:7" s="2" customFormat="1">
+      <c r="G75" s="26"/>
+      <c r="H75" s="20"/>
+    </row>
+    <row r="76" spans="3:8" s="2" customFormat="1">
       <c r="C76" s="20"/>
-      <c r="D76" s="26"/>
+      <c r="D76" s="30"/>
       <c r="E76" s="26"/>
       <c r="F76" s="26"/>
-      <c r="G76" s="20"/>
-    </row>
-    <row r="77" spans="3:7" s="2" customFormat="1">
+      <c r="G76" s="26"/>
+      <c r="H76" s="20"/>
+    </row>
+    <row r="77" spans="3:8" s="2" customFormat="1">
       <c r="C77" s="20"/>
-      <c r="D77" s="26"/>
+      <c r="D77" s="30"/>
       <c r="E77" s="26"/>
       <c r="F77" s="26"/>
-      <c r="G77" s="20"/>
-    </row>
-    <row r="78" spans="3:7" s="2" customFormat="1">
+      <c r="G77" s="26"/>
+      <c r="H77" s="20"/>
+    </row>
+    <row r="78" spans="3:8" s="2" customFormat="1">
       <c r="C78" s="20"/>
-      <c r="D78" s="26"/>
+      <c r="D78" s="30"/>
       <c r="E78" s="26"/>
       <c r="F78" s="26"/>
-      <c r="G78" s="20"/>
-    </row>
-    <row r="79" spans="3:7" s="2" customFormat="1">
+      <c r="G78" s="26"/>
+      <c r="H78" s="20"/>
+    </row>
+    <row r="79" spans="3:8" s="2" customFormat="1">
       <c r="C79" s="20"/>
-      <c r="D79" s="26"/>
+      <c r="D79" s="30"/>
       <c r="E79" s="26"/>
       <c r="F79" s="26"/>
-      <c r="G79" s="20"/>
-    </row>
-    <row r="80" spans="3:7" s="2" customFormat="1">
+      <c r="G79" s="26"/>
+      <c r="H79" s="20"/>
+    </row>
+    <row r="80" spans="3:8" s="2" customFormat="1">
       <c r="C80" s="20"/>
-      <c r="D80" s="26"/>
+      <c r="D80" s="30"/>
       <c r="E80" s="26"/>
       <c r="F80" s="26"/>
-      <c r="G80" s="20"/>
-    </row>
-    <row r="81" spans="3:7" s="2" customFormat="1">
+      <c r="G80" s="26"/>
+      <c r="H80" s="20"/>
+    </row>
+    <row r="81" spans="3:8" s="2" customFormat="1">
       <c r="C81" s="20"/>
-      <c r="D81" s="26"/>
+      <c r="D81" s="30"/>
       <c r="E81" s="26"/>
       <c r="F81" s="26"/>
-      <c r="G81" s="20"/>
-    </row>
-    <row r="82" spans="3:7" s="2" customFormat="1">
+      <c r="G81" s="26"/>
+      <c r="H81" s="20"/>
+    </row>
+    <row r="82" spans="3:8" s="2" customFormat="1">
       <c r="C82" s="20"/>
-      <c r="D82" s="26"/>
+      <c r="D82" s="30"/>
       <c r="E82" s="26"/>
       <c r="F82" s="26"/>
-      <c r="G82" s="20"/>
-    </row>
-    <row r="83" spans="3:7" s="2" customFormat="1">
+      <c r="G82" s="26"/>
+      <c r="H82" s="20"/>
+    </row>
+    <row r="83" spans="3:8" s="2" customFormat="1">
       <c r="C83" s="20"/>
-      <c r="D83" s="26"/>
+      <c r="D83" s="30"/>
       <c r="E83" s="26"/>
       <c r="F83" s="26"/>
-      <c r="G83" s="20"/>
-    </row>
-    <row r="84" spans="3:7" s="2" customFormat="1">
+      <c r="G83" s="26"/>
+      <c r="H83" s="20"/>
+    </row>
+    <row r="84" spans="3:8" s="2" customFormat="1">
       <c r="C84" s="20"/>
-      <c r="D84" s="26"/>
+      <c r="D84" s="30"/>
       <c r="E84" s="26"/>
       <c r="F84" s="26"/>
-      <c r="G84" s="20"/>
-    </row>
-    <row r="85" spans="3:7" s="2" customFormat="1">
+      <c r="G84" s="26"/>
+      <c r="H84" s="20"/>
+    </row>
+    <row r="85" spans="3:8" s="2" customFormat="1">
       <c r="C85" s="20"/>
-      <c r="D85" s="26"/>
+      <c r="D85" s="30"/>
       <c r="E85" s="26"/>
       <c r="F85" s="26"/>
-      <c r="G85" s="20"/>
-    </row>
-    <row r="86" spans="3:7" s="2" customFormat="1">
+      <c r="G85" s="26"/>
+      <c r="H85" s="20"/>
+    </row>
+    <row r="86" spans="3:8" s="2" customFormat="1">
       <c r="C86" s="20"/>
-      <c r="D86" s="26"/>
+      <c r="D86" s="30"/>
       <c r="E86" s="26"/>
       <c r="F86" s="26"/>
-      <c r="G86" s="20"/>
-    </row>
-    <row r="87" spans="3:7" s="2" customFormat="1">
+      <c r="G86" s="26"/>
+      <c r="H86" s="20"/>
+    </row>
+    <row r="87" spans="3:8" s="2" customFormat="1">
       <c r="C87" s="20"/>
-      <c r="D87" s="26"/>
+      <c r="D87" s="30"/>
       <c r="E87" s="26"/>
       <c r="F87" s="26"/>
-      <c r="G87" s="20"/>
-    </row>
-    <row r="88" spans="3:7" s="2" customFormat="1">
+      <c r="G87" s="26"/>
+      <c r="H87" s="20"/>
+    </row>
+    <row r="88" spans="3:8" s="2" customFormat="1">
       <c r="C88" s="20"/>
-      <c r="D88" s="26"/>
+      <c r="D88" s="30"/>
       <c r="E88" s="26"/>
       <c r="F88" s="26"/>
-      <c r="G88" s="20"/>
-    </row>
-    <row r="89" spans="3:7" s="2" customFormat="1">
+      <c r="G88" s="26"/>
+      <c r="H88" s="20"/>
+    </row>
+    <row r="89" spans="3:8" s="2" customFormat="1">
       <c r="C89" s="20"/>
-      <c r="D89" s="26"/>
+      <c r="D89" s="30"/>
       <c r="E89" s="26"/>
       <c r="F89" s="26"/>
-      <c r="G89" s="20"/>
-    </row>
-    <row r="90" spans="3:7" s="2" customFormat="1">
+      <c r="G89" s="26"/>
+      <c r="H89" s="20"/>
+    </row>
+    <row r="90" spans="3:8" s="2" customFormat="1">
       <c r="C90" s="20"/>
-      <c r="D90" s="26"/>
+      <c r="D90" s="30"/>
       <c r="E90" s="26"/>
       <c r="F90" s="26"/>
-      <c r="G90" s="20"/>
-    </row>
-    <row r="91" spans="3:7" s="2" customFormat="1">
+      <c r="G90" s="26"/>
+      <c r="H90" s="20"/>
+    </row>
+    <row r="91" spans="3:8" s="2" customFormat="1">
       <c r="C91" s="20"/>
-      <c r="D91" s="26"/>
+      <c r="D91" s="30"/>
       <c r="E91" s="26"/>
       <c r="F91" s="26"/>
-      <c r="G91" s="20"/>
-    </row>
-    <row r="92" spans="3:7" s="2" customFormat="1">
+      <c r="G91" s="26"/>
+      <c r="H91" s="20"/>
+    </row>
+    <row r="92" spans="3:8" s="2" customFormat="1">
       <c r="C92" s="20"/>
-      <c r="D92" s="26"/>
+      <c r="D92" s="30"/>
       <c r="E92" s="26"/>
       <c r="F92" s="26"/>
-      <c r="G92" s="20"/>
-    </row>
-    <row r="93" spans="3:7" s="2" customFormat="1">
+      <c r="G92" s="26"/>
+      <c r="H92" s="20"/>
+    </row>
+    <row r="93" spans="3:8" s="2" customFormat="1">
       <c r="C93" s="20"/>
-      <c r="D93" s="26"/>
+      <c r="D93" s="30"/>
       <c r="E93" s="26"/>
       <c r="F93" s="26"/>
-      <c r="G93" s="20"/>
-    </row>
-    <row r="94" spans="3:7" s="2" customFormat="1">
+      <c r="G93" s="26"/>
+      <c r="H93" s="20"/>
+    </row>
+    <row r="94" spans="3:8" s="2" customFormat="1">
       <c r="C94" s="20"/>
-      <c r="D94" s="26"/>
+      <c r="D94" s="30"/>
       <c r="E94" s="26"/>
       <c r="F94" s="26"/>
-      <c r="G94" s="20"/>
-    </row>
-    <row r="95" spans="3:7" s="2" customFormat="1">
+      <c r="G94" s="26"/>
+      <c r="H94" s="20"/>
+    </row>
+    <row r="95" spans="3:8" s="2" customFormat="1">
       <c r="C95" s="20"/>
-      <c r="D95" s="26"/>
+      <c r="D95" s="30"/>
       <c r="E95" s="26"/>
       <c r="F95" s="26"/>
-      <c r="G95" s="20"/>
-    </row>
-    <row r="96" spans="3:7" s="2" customFormat="1">
+      <c r="G95" s="26"/>
+      <c r="H95" s="20"/>
+    </row>
+    <row r="96" spans="3:8" s="2" customFormat="1">
       <c r="C96" s="20"/>
-      <c r="D96" s="26"/>
+      <c r="D96" s="30"/>
       <c r="E96" s="26"/>
       <c r="F96" s="26"/>
-      <c r="G96" s="20"/>
-    </row>
-    <row r="97" spans="3:7" s="2" customFormat="1">
+      <c r="G96" s="26"/>
+      <c r="H96" s="20"/>
+    </row>
+    <row r="97" spans="3:8" s="2" customFormat="1">
       <c r="C97" s="20"/>
-      <c r="D97" s="26"/>
+      <c r="D97" s="30"/>
       <c r="E97" s="26"/>
       <c r="F97" s="26"/>
-      <c r="G97" s="20"/>
-    </row>
-    <row r="98" spans="3:7" s="2" customFormat="1">
+      <c r="G97" s="26"/>
+      <c r="H97" s="20"/>
+    </row>
+    <row r="98" spans="3:8" s="2" customFormat="1">
       <c r="C98" s="20"/>
-      <c r="D98" s="26"/>
+      <c r="D98" s="30"/>
       <c r="E98" s="26"/>
       <c r="F98" s="26"/>
-      <c r="G98" s="20"/>
-    </row>
-    <row r="99" spans="3:7" s="2" customFormat="1">
+      <c r="G98" s="26"/>
+      <c r="H98" s="20"/>
+    </row>
+    <row r="99" spans="3:8" s="2" customFormat="1">
       <c r="C99" s="20"/>
-      <c r="D99" s="26"/>
+      <c r="D99" s="30"/>
       <c r="E99" s="26"/>
       <c r="F99" s="26"/>
-      <c r="G99" s="20"/>
-    </row>
-    <row r="100" spans="3:7" s="2" customFormat="1">
+      <c r="G99" s="26"/>
+      <c r="H99" s="20"/>
+    </row>
+    <row r="100" spans="3:8" s="2" customFormat="1">
       <c r="C100" s="20"/>
-      <c r="D100" s="26"/>
+      <c r="D100" s="30"/>
       <c r="E100" s="26"/>
       <c r="F100" s="26"/>
-      <c r="G100" s="20"/>
-    </row>
-    <row r="101" spans="3:7" s="2" customFormat="1">
+      <c r="G100" s="26"/>
+      <c r="H100" s="20"/>
+    </row>
+    <row r="101" spans="3:8" s="2" customFormat="1">
       <c r="C101" s="20"/>
-      <c r="D101" s="26"/>
+      <c r="D101" s="30"/>
       <c r="E101" s="26"/>
       <c r="F101" s="26"/>
-      <c r="G101" s="20"/>
-    </row>
-    <row r="102" spans="3:7" s="2" customFormat="1">
+      <c r="G101" s="26"/>
+      <c r="H101" s="20"/>
+    </row>
+    <row r="102" spans="3:8" s="2" customFormat="1">
       <c r="C102" s="20"/>
-      <c r="D102" s="26"/>
+      <c r="D102" s="30"/>
       <c r="E102" s="26"/>
       <c r="F102" s="26"/>
-      <c r="G102" s="20"/>
-    </row>
-    <row r="103" spans="3:7" s="2" customFormat="1">
+      <c r="G102" s="26"/>
+      <c r="H102" s="20"/>
+    </row>
+    <row r="103" spans="3:8" s="2" customFormat="1">
       <c r="C103" s="20"/>
-      <c r="D103" s="26"/>
+      <c r="D103" s="30"/>
       <c r="E103" s="26"/>
       <c r="F103" s="26"/>
-      <c r="G103" s="20"/>
-    </row>
-    <row r="104" spans="3:7" s="2" customFormat="1">
+      <c r="G103" s="26"/>
+      <c r="H103" s="20"/>
+    </row>
+    <row r="104" spans="3:8" s="2" customFormat="1">
       <c r="C104" s="20"/>
-      <c r="D104" s="26"/>
+      <c r="D104" s="30"/>
       <c r="E104" s="26"/>
       <c r="F104" s="26"/>
-      <c r="G104" s="20"/>
-    </row>
-    <row r="105" spans="3:7" s="2" customFormat="1">
+      <c r="G104" s="26"/>
+      <c r="H104" s="20"/>
+    </row>
+    <row r="105" spans="3:8" s="2" customFormat="1">
       <c r="C105" s="20"/>
-      <c r="D105" s="26"/>
+      <c r="D105" s="30"/>
       <c r="E105" s="26"/>
       <c r="F105" s="26"/>
-      <c r="G105" s="20"/>
-    </row>
-    <row r="106" spans="3:7" s="2" customFormat="1">
+      <c r="G105" s="26"/>
+      <c r="H105" s="20"/>
+    </row>
+    <row r="106" spans="3:8" s="2" customFormat="1">
       <c r="C106" s="20"/>
-      <c r="D106" s="26"/>
+      <c r="D106" s="30"/>
       <c r="E106" s="26"/>
       <c r="F106" s="26"/>
-      <c r="G106" s="20"/>
+      <c r="G106" s="26"/>
+      <c r="H106" s="20"/>
     </row>
   </sheetData>
   <sortState columnSort="1" ref="C1:S24">
@@ -2368,8 +2653,8 @@
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFCFCFF"/>
+        <color rgb="FF53FF88"/>
+        <color rgb="FFFF0000"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
merge updates on master.
</commit_message>
<xml_diff>
--- a/INRC2_Simulator/log/TestedParameter.xlsx
+++ b/INRC2_Simulator/log/TestedParameter.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\NurseRosteringProblem\INRC2_Simulator\log\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\cpp\NurseRostering\INRC2_Simulator\log\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="64080" yWindow="0" windowWidth="14145" windowHeight="5115"/>
+    <workbookView xWindow="67320" yWindow="0" windowWidth="14145" windowHeight="5115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="37">
   <si>
     <t>TableSize</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -167,6 +167,10 @@
   </si>
   <si>
     <t>0524</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Final Release</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -177,7 +181,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,6 +208,15 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -238,7 +251,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -341,12 +354,12 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -357,119 +370,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF7C80"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF33CC33"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -756,7 +666,7 @@
       <pane xSplit="2" ySplit="19" topLeftCell="C20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A13" sqref="A13"/>
-      <selection pane="bottomRight" activeCell="K18" sqref="K18"/>
+      <selection pane="bottomRight" activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="13.5"/>
@@ -1855,10 +1765,10 @@
         <v>7</v>
       </c>
       <c r="B19" s="37"/>
-      <c r="C19" s="34" t="s">
+      <c r="C19" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="35" t="s">
+      <c r="D19" s="34" t="s">
         <v>34</v>
       </c>
       <c r="E19" s="26" t="s">
@@ -1867,7 +1777,7 @@
       <c r="F19" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="G19" s="34" t="s">
+      <c r="G19" s="35" t="s">
         <v>34</v>
       </c>
       <c r="H19" s="20" t="s">
@@ -1913,13 +1823,15 @@
     <row r="20" spans="1:20" s="2" customFormat="1">
       <c r="C20" s="20"/>
       <c r="D20" s="30"/>
-      <c r="E20" s="35" t="s">
+      <c r="E20" s="34" t="s">
         <v>34</v>
       </c>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
       <c r="H20" s="20"/>
-      <c r="I20" s="26"/>
+      <c r="I20" s="40" t="s">
+        <v>36</v>
+      </c>
       <c r="K20" s="23" t="s">
         <v>29</v>
       </c>

</xml_diff>